<commit_message>
Update Coal phase out announcements.xlsx
</commit_message>
<xml_diff>
--- a/Other data/Coal phase out announcements.xlsx
+++ b/Other data/Coal phase out announcements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive - London School of Economics\Documents\LSE\GY489_Dissertation\LETS GO\Dissertation-Code-Data\Other data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFAD611-C0CA-4113-B4BC-6EFDB2C6AF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D344B222-7128-48EE-9F37-8187B6E30D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="21585" windowHeight="13665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -671,7 +671,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -745,118 +745,139 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="9">
-        <v>42326</v>
+      <c r="A2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43358</v>
       </c>
       <c r="C2" s="2">
-        <v>2025</v>
+        <v>2038</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F2" s="2">
-        <v>21.2</v>
-      </c>
-      <c r="G2" s="1">
-        <v>43105</v>
-      </c>
-      <c r="H2">
-        <v>2025</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
+        <v>47.6</v>
+      </c>
+      <c r="G2" s="9">
+        <v>43491</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2038</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="J2" s="1">
-        <v>44179</v>
-      </c>
-      <c r="K2">
-        <v>2024</v>
+        <v>43846</v>
       </c>
       <c r="L2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="1"/>
-      <c r="S2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T2" t="s">
-        <v>21</v>
+        <v>64</v>
+      </c>
+      <c r="M2" s="1">
+        <v>44484</v>
+      </c>
+      <c r="N2">
+        <v>2030</v>
+      </c>
+      <c r="O2" t="s">
+        <v>66</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1">
-        <v>42486</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="9">
+        <v>42326</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2025</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F3" s="2">
-        <v>5.8</v>
-      </c>
-      <c r="G3" s="9">
-        <v>42689</v>
-      </c>
-      <c r="H3" s="2">
-        <v>2023</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
+        <v>21.2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>43105</v>
+      </c>
+      <c r="H3">
+        <v>2025</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
       </c>
       <c r="J3" s="1">
-        <v>42922</v>
-      </c>
-      <c r="K3" s="2">
-        <v>2022</v>
+        <v>44179</v>
+      </c>
+      <c r="K3">
+        <v>2024</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="S3" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="T3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="7">
-        <v>43032</v>
+      <c r="A4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="9">
+        <v>43419</v>
       </c>
       <c r="C4" s="2">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F4" s="2">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="G4" s="1">
-        <v>43731</v>
+        <v>10.5</v>
+      </c>
+      <c r="G4" s="10">
+        <v>43518</v>
       </c>
       <c r="H4" s="2">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="T4" t="s">
-        <v>21</v>
+        <v>72</v>
+      </c>
+      <c r="J4" s="1">
+        <v>43850</v>
+      </c>
+      <c r="K4">
+        <v>2030</v>
+      </c>
+      <c r="L4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M4" s="1">
+        <v>44377</v>
+      </c>
+      <c r="O4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.45">
@@ -940,38 +961,34 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="1">
-        <v>42636</v>
-      </c>
-      <c r="C7"/>
-      <c r="D7" t="s">
-        <v>41</v>
+        <v>19</v>
+      </c>
+      <c r="B7" s="7">
+        <v>43032</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2025</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" s="2">
-        <v>6.3</v>
-      </c>
-      <c r="G7" s="9">
-        <v>43018</v>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G7" s="1">
+        <v>43731</v>
       </c>
       <c r="H7" s="2">
-        <v>2030</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="1">
-        <v>43238</v>
-      </c>
-      <c r="K7" s="2">
-        <v>2029</v>
-      </c>
-      <c r="L7" t="s">
-        <v>42</v>
+        <v>2025</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="T7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.45">
@@ -1024,40 +1041,31 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="9">
-        <v>43731</v>
+        <v>85</v>
+      </c>
+      <c r="B11" s="7">
+        <v>44169</v>
       </c>
       <c r="C11" s="2">
-        <v>2028</v>
+        <v>2038</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F11" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G11" s="1">
-        <v>44462</v>
+        <v>8.5</v>
+      </c>
+      <c r="G11" s="7">
+        <v>44568</v>
       </c>
       <c r="H11" s="2">
-        <v>2025</v>
+        <v>2033</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
-      </c>
-      <c r="J11" s="1">
-        <v>44657</v>
-      </c>
-      <c r="K11">
-        <v>2028</v>
-      </c>
-      <c r="L11" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.45">
@@ -1101,50 +1109,39 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A14" s="4" t="s">
-        <v>62</v>
+      <c r="A14" t="s">
+        <v>39</v>
       </c>
       <c r="B14" s="1">
-        <v>43358</v>
-      </c>
-      <c r="C14" s="2">
-        <v>2038</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>65</v>
+        <v>42636</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14" t="s">
+        <v>41</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2">
-        <v>47.6</v>
+        <v>6.3</v>
       </c>
       <c r="G14" s="9">
-        <v>43491</v>
+        <v>43018</v>
       </c>
       <c r="H14" s="2">
-        <v>2038</v>
+        <v>2030</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="J14" s="1">
-        <v>43846</v>
+        <v>43238</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2029</v>
       </c>
       <c r="L14" t="s">
-        <v>64</v>
-      </c>
-      <c r="M14" s="1">
-        <v>44484</v>
-      </c>
-      <c r="N14">
-        <v>2030</v>
-      </c>
-      <c r="O14" t="s">
-        <v>66</v>
-      </c>
-      <c r="S14" s="6" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.45">
@@ -1168,47 +1165,41 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A16" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="9">
-        <v>43419</v>
-      </c>
-      <c r="C16" s="2">
-        <v>2030</v>
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>42486</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="2">
-        <v>10.5</v>
-      </c>
-      <c r="G16" s="10">
-        <v>43518</v>
+        <v>5.8</v>
+      </c>
+      <c r="G16" s="9">
+        <v>42689</v>
       </c>
       <c r="H16" s="2">
-        <v>2030</v>
-      </c>
-      <c r="I16" t="s">
-        <v>72</v>
+        <v>2023</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="J16" s="1">
-        <v>43850</v>
-      </c>
-      <c r="K16">
-        <v>2030</v>
+        <v>42922</v>
+      </c>
+      <c r="K16" s="2">
+        <v>2022</v>
       </c>
       <c r="L16" t="s">
-        <v>73</v>
-      </c>
-      <c r="M16" s="1">
-        <v>44377</v>
-      </c>
-      <c r="O16" t="s">
-        <v>74</v>
+        <v>18</v>
+      </c>
+      <c r="T16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
@@ -1310,31 +1301,40 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B22" s="7">
-        <v>44169</v>
+        <v>54</v>
+      </c>
+      <c r="B22" s="9">
+        <v>43731</v>
       </c>
       <c r="C22" s="2">
-        <v>2038</v>
+        <v>2028</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" s="2">
-        <v>8.5</v>
-      </c>
-      <c r="G22" s="7">
-        <v>44568</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G22" s="1">
+        <v>44462</v>
       </c>
       <c r="H22" s="2">
-        <v>2033</v>
+        <v>2025</v>
       </c>
       <c r="I22" t="s">
-        <v>87</v>
+        <v>55</v>
+      </c>
+      <c r="J22" s="1">
+        <v>44657</v>
+      </c>
+      <c r="K22">
+        <v>2028</v>
+      </c>
+      <c r="L22" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:19" hidden="1" x14ac:dyDescent="0.45">
@@ -1356,6 +1356,9 @@
         <filter val="yes"/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T22">
+      <sortCondition descending="1" ref="F1:F23"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
new file; just a check
</commit_message>
<xml_diff>
--- a/Other data/Coal phase out announcements.xlsx
+++ b/Other data/Coal phase out announcements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive - London School of Economics\Documents\LSE\GY489_Dissertation\LETS GO\Dissertation-Code-Data\Other data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44AE399-B6A1-41F5-8272-3D69FE00AE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15171072-9B7A-41C3-A797-D3E8EAB2575C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="356">
   <si>
     <t>Country</t>
   </si>
@@ -1138,13 +1138,16 @@
   <si>
     <t xml:space="preserve">Energy state secretary announces 2025 phase-out; 22: company announces it </t>
   </si>
+  <si>
+    <t>confounding event CP: expectations of post 2020 ETS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyymmdd"/>
+    <numFmt numFmtId="164" formatCode="yyyymmdd"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -1279,10 +1282,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2344,10 +2347,10 @@
   <dimension ref="A1:R76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2426,1183 +2429,1183 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="P2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+      <c r="B2" s="14">
+        <v>40872</v>
+      </c>
+      <c r="F2">
+        <v>2030</v>
+      </c>
+      <c r="R2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E3"/>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="11">
-        <v>44480</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>15</v>
-      </c>
-      <c r="L4">
+        <v>36</v>
+      </c>
+      <c r="B3" s="14">
+        <v>41941</v>
+      </c>
+      <c r="D3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G3">
+        <v>2.5</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="L3">
         <v>1</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="R3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="16">
+        <v>42283</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
-      <c r="O4" t="s">
-        <v>153</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>126</v>
-      </c>
       <c r="R4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="15">
-        <v>44483</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" t="s">
-        <v>131</v>
-      </c>
-      <c r="G5">
-        <v>5</v>
-      </c>
-      <c r="H5">
-        <v>15</v>
-      </c>
-      <c r="L5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="11">
+        <v>42326</v>
+      </c>
+      <c r="R5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="16">
+        <v>42636</v>
+      </c>
+      <c r="P6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="14">
+        <v>42689</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F7">
+        <v>2023</v>
+      </c>
+      <c r="G7">
+        <v>3.5</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>137</v>
+      </c>
+      <c r="L7">
         <v>1</v>
       </c>
-      <c r="N5">
+      <c r="N7">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6">
-        <v>0.3</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7"/>
-      <c r="M7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="P7" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="R7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="15">
-        <v>44169</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F8">
-        <v>2038</v>
+        <v>24</v>
+      </c>
+      <c r="B8" s="16">
+        <v>42697</v>
       </c>
       <c r="G8">
-        <v>8.5</v>
+        <v>2.6</v>
       </c>
       <c r="H8">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
-      <c r="N8">
+      <c r="P8" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="R8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="14">
+        <v>42978</v>
+      </c>
+      <c r="E9"/>
+      <c r="R9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="14">
+        <v>42996</v>
+      </c>
+      <c r="R10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="15">
+        <v>43018</v>
+      </c>
+      <c r="N11">
         <v>1</v>
       </c>
-      <c r="R8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="11">
-        <v>44568</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="N9">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="15">
+        <v>43032</v>
+      </c>
+      <c r="N12">
         <v>1</v>
       </c>
-      <c r="R9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="R12" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="11">
+        <v>43049</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="R13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="14">
-        <v>40872</v>
-      </c>
-      <c r="F10">
-        <v>2030</v>
-      </c>
-      <c r="R10" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="14">
-        <v>41941</v>
-      </c>
-      <c r="D11" t="s">
-        <v>196</v>
-      </c>
-      <c r="G11">
-        <v>2.5</v>
-      </c>
-      <c r="H11">
-        <v>6</v>
-      </c>
-      <c r="L11">
+      <c r="B14" s="14">
+        <v>43055</v>
+      </c>
+      <c r="D14" t="s">
+        <v>198</v>
+      </c>
+      <c r="K14" t="s">
+        <v>199</v>
+      </c>
+      <c r="R14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="14">
+        <v>43055</v>
+      </c>
+      <c r="D15" t="s">
+        <v>211</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+      <c r="K15" t="s">
+        <v>138</v>
+      </c>
+      <c r="L15">
         <v>1</v>
       </c>
-      <c r="P11" s="6" t="s">
+      <c r="P15" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="R11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="14">
-        <v>43055</v>
-      </c>
-      <c r="D12" t="s">
-        <v>198</v>
-      </c>
-      <c r="K12" t="s">
-        <v>199</v>
-      </c>
-      <c r="R12" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13"/>
-      <c r="M13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="16">
-        <v>42697</v>
-      </c>
-      <c r="G14">
-        <v>2.6</v>
-      </c>
-      <c r="H14">
-        <v>6</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="R14" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="14">
-        <v>42978</v>
-      </c>
-      <c r="E15"/>
       <c r="R15" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="14">
-        <v>43200</v>
-      </c>
-      <c r="E16"/>
+      <c r="A16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="16">
+        <v>43091</v>
+      </c>
+      <c r="D16" t="s">
+        <v>215</v>
+      </c>
+      <c r="P16" s="6"/>
       <c r="R16" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>24</v>
+      <c r="A17" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B17" s="14">
-        <v>43391</v>
-      </c>
-      <c r="E17"/>
+        <v>43105</v>
+      </c>
       <c r="R17" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="16">
+        <v>43169</v>
+      </c>
+      <c r="G18">
+        <v>0.9</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="N18" t="s">
+        <v>52</v>
+      </c>
+      <c r="R18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="14">
-        <v>43523</v>
-      </c>
-      <c r="E18"/>
-      <c r="R18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
       <c r="B19" s="14">
-        <v>42689</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="F19">
-        <v>2023</v>
-      </c>
-      <c r="G19">
-        <v>3.5</v>
-      </c>
-      <c r="H19">
-        <v>11</v>
-      </c>
-      <c r="K19" t="s">
-        <v>137</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="P19" s="6" t="s">
-        <v>135</v>
-      </c>
+        <v>43200</v>
+      </c>
+      <c r="E19"/>
       <c r="R19" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="11">
-        <v>43357</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20">
-        <v>2038</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="6" t="s">
-        <v>108</v>
+      <c r="A20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="14">
+        <v>43238</v>
       </c>
       <c r="R20" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="15">
-        <v>43491</v>
+      <c r="B21" s="11">
+        <v>43357</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F21">
         <v>2038</v>
       </c>
-      <c r="G21">
-        <v>47.6</v>
-      </c>
-      <c r="H21">
-        <v>175</v>
-      </c>
       <c r="L21">
         <v>1</v>
       </c>
       <c r="N21">
         <v>1</v>
       </c>
-      <c r="P21" s="6"/>
+      <c r="Q21" s="6" t="s">
+        <v>108</v>
+      </c>
       <c r="R21" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="11">
-        <v>43846</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22">
-        <v>2038</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="P22" s="6"/>
+        <v>24</v>
+      </c>
+      <c r="B22" s="14">
+        <v>43391</v>
+      </c>
+      <c r="E22"/>
       <c r="R22" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="11">
-        <v>44015</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F23">
-        <v>2038</v>
-      </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="P23" s="6"/>
-      <c r="R23" t="s">
-        <v>160</v>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="14">
+        <v>43397</v>
+      </c>
+      <c r="P23" s="6" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="11">
-        <v>44484</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F24">
-        <v>2030</v>
+      <c r="A24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="14">
+        <v>43419</v>
       </c>
       <c r="N24">
         <v>1</v>
       </c>
-      <c r="P24" s="6" t="s">
-        <v>146</v>
+      <c r="P24" t="s">
+        <v>184</v>
       </c>
       <c r="R24" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="11">
-        <v>44705</v>
+      <c r="A25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="14">
+        <v>43423</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="6"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
+        <v>217</v>
+      </c>
+      <c r="P25" s="6"/>
+      <c r="R25" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="11">
-        <v>44732</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="6"/>
+        <v>56</v>
+      </c>
+      <c r="B26" s="16">
+        <v>43424</v>
+      </c>
+      <c r="G26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>194</v>
+      </c>
       <c r="R26" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>167</v>
+      <c r="B27" s="15">
+        <v>43491</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27">
+        <v>2038</v>
+      </c>
+      <c r="G27">
+        <v>47.6</v>
+      </c>
+      <c r="H27">
+        <v>175</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
       </c>
       <c r="P27" s="6"/>
       <c r="R27" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="15">
-        <v>43731</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F28">
-        <v>2028</v>
-      </c>
-      <c r="K28" t="s">
-        <v>148</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
-      <c r="P28" s="6" t="s">
-        <v>166</v>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="18">
+        <v>43497</v>
+      </c>
+      <c r="G28">
+        <v>0.7</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
       </c>
       <c r="R28" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>53</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A29" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="B29" s="14">
-        <v>44312</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F29">
-        <v>2025</v>
-      </c>
-      <c r="P29" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q29" s="6"/>
+        <v>43518</v>
+      </c>
       <c r="R29" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="B30" s="14">
-        <v>44462</v>
-      </c>
+        <v>43523</v>
+      </c>
+      <c r="E30"/>
       <c r="R30" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="19">
+        <v>43634</v>
+      </c>
+      <c r="D31" t="s">
+        <v>220</v>
+      </c>
+      <c r="R31" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A32" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="16">
-        <v>44530</v>
-      </c>
-      <c r="Q31" s="6"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" s="14">
-        <v>44657</v>
+      <c r="B32" s="15">
+        <v>43731</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F32">
         <v>2028</v>
       </c>
-      <c r="P32" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q32" s="6"/>
-    </row>
-    <row r="33" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="K32" t="s">
+        <v>148</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="R32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="16">
-        <v>43424</v>
-      </c>
-      <c r="G33">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H33">
-        <v>4</v>
-      </c>
-      <c r="P33" s="6" t="s">
-        <v>194</v>
-      </c>
+      <c r="B33" s="14">
+        <v>43731</v>
+      </c>
+      <c r="Q33" s="6"/>
       <c r="R33" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="14">
+      <c r="A34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="16">
         <v>43731</v>
-      </c>
-      <c r="Q34" s="6"/>
-      <c r="R34" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>42</v>
+      </c>
+      <c r="B35" s="14">
+        <v>43764</v>
       </c>
       <c r="E35"/>
-      <c r="M35">
-        <v>0</v>
+      <c r="R35" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>44</v>
+      <c r="A36" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B36" s="16">
-        <v>43169</v>
-      </c>
-      <c r="G36">
-        <v>0.9</v>
-      </c>
-      <c r="H36">
-        <v>2</v>
-      </c>
-      <c r="N36" t="s">
-        <v>52</v>
-      </c>
-      <c r="R36" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A37" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B37" s="15">
-        <v>43032</v>
+        <v>43802</v>
+      </c>
+      <c r="P36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="11">
+        <v>43846</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37">
+        <v>2038</v>
       </c>
       <c r="N37">
         <v>1</v>
       </c>
-      <c r="R37" s="17" t="s">
-        <v>168</v>
+      <c r="P37" s="6"/>
+      <c r="R37" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="11">
-        <v>43049</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>169</v>
+        <v>69</v>
+      </c>
+      <c r="B38" s="16">
+        <v>43850</v>
       </c>
       <c r="R38" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A39" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="16">
-        <v>43731</v>
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="11">
+        <v>44015</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F39">
+        <v>2038</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="P39" s="6"/>
+      <c r="R39" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>82</v>
+      </c>
+      <c r="B40" s="11">
+        <v>44099</v>
       </c>
       <c r="E40"/>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
+      <c r="F40">
+        <v>2049</v>
+      </c>
+      <c r="G40">
+        <v>30.2</v>
+      </c>
+      <c r="H40">
+        <v>104</v>
+      </c>
+      <c r="R40" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>119</v>
-      </c>
-      <c r="M41">
-        <v>0</v>
+        <v>84</v>
+      </c>
+      <c r="B41" s="15">
+        <v>44169</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F41">
+        <v>2038</v>
+      </c>
+      <c r="G41">
+        <v>8.5</v>
+      </c>
+      <c r="H41">
+        <v>35</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
       </c>
       <c r="N41">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="R41" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>113</v>
-      </c>
-      <c r="E42"/>
-      <c r="M42">
-        <v>0</v>
-      </c>
-      <c r="N42">
-        <v>0</v>
+      <c r="A42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="11">
+        <v>44179</v>
+      </c>
+      <c r="R42" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>115</v>
-      </c>
-      <c r="M43">
-        <v>0</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+      <c r="B43" s="14">
+        <v>44270</v>
+      </c>
+      <c r="D43" t="s">
+        <v>323</v>
+      </c>
+      <c r="E43"/>
+      <c r="R43" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>117</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
-      <c r="N44">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="B44" s="14">
+        <v>44312</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F44">
+        <v>2025</v>
+      </c>
+      <c r="P44" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q44" s="6"/>
+      <c r="R44" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="16">
-        <v>42636</v>
-      </c>
-      <c r="P45" t="s">
-        <v>172</v>
+        <v>76</v>
+      </c>
+      <c r="B45" s="14">
+        <v>44342</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="R45" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B46" s="15">
-        <v>43018</v>
-      </c>
-      <c r="N46">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="B46" s="11">
+        <v>44350</v>
+      </c>
+      <c r="P46" s="6"/>
+      <c r="R46" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="B47" s="14">
-        <v>43238</v>
+        <v>44377</v>
       </c>
       <c r="R47" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B48" s="16">
-        <v>43802</v>
-      </c>
-      <c r="P48" t="s">
-        <v>171</v>
+        <v>8</v>
+      </c>
+      <c r="B48" s="14">
+        <v>44377</v>
+      </c>
+      <c r="R48" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A49" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>173</v>
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="14">
+        <v>44462</v>
       </c>
       <c r="R49" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>120</v>
-      </c>
-      <c r="E50"/>
-      <c r="M50">
-        <v>0</v>
-      </c>
-      <c r="N50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A50" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="16">
+        <v>44469</v>
+      </c>
+      <c r="P50" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="85.5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B51" s="11">
-        <v>44099</v>
-      </c>
-      <c r="E51"/>
-      <c r="F51">
-        <v>2049</v>
+        <v>44480</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F51" t="s">
+        <v>127</v>
       </c>
       <c r="G51">
-        <v>30.2</v>
+        <v>5</v>
       </c>
       <c r="H51">
-        <v>104</v>
+        <v>15</v>
+      </c>
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51" t="s">
+        <v>153</v>
+      </c>
+      <c r="P51" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q51" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="R51" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>42</v>
-      </c>
-      <c r="B52" s="14">
-        <v>43055</v>
-      </c>
-      <c r="D52" t="s">
-        <v>211</v>
+        <v>80</v>
+      </c>
+      <c r="B52" s="15">
+        <v>44483</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F52" t="s">
+        <v>131</v>
       </c>
       <c r="G52">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H52">
-        <v>12</v>
-      </c>
-      <c r="K52" t="s">
-        <v>138</v>
+        <v>15</v>
       </c>
       <c r="L52">
         <v>1</v>
       </c>
-      <c r="P52" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="R52" t="s">
-        <v>212</v>
+      <c r="N52">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>42</v>
-      </c>
-      <c r="B53" s="14">
-        <v>43764</v>
-      </c>
-      <c r="E53"/>
+        <v>61</v>
+      </c>
+      <c r="B53" s="11">
+        <v>44484</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F53">
+        <v>2030</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="P53" s="6" t="s">
+        <v>146</v>
+      </c>
       <c r="R53" t="s">
-        <v>213</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A54" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B54" s="16">
+        <v>44504</v>
+      </c>
+      <c r="D54" t="s">
+        <v>320</v>
+      </c>
+      <c r="P54" t="s">
+        <v>224</v>
+      </c>
+      <c r="R54" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="16">
+        <v>44530</v>
+      </c>
+      <c r="Q55" s="6"/>
+    </row>
+    <row r="56" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="11">
+        <v>44568</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="R56" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="11">
+        <v>44574</v>
+      </c>
+      <c r="G57">
+        <v>1.5</v>
+      </c>
+      <c r="H57">
+        <v>5</v>
+      </c>
+      <c r="R57" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" s="14">
+        <v>44657</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F58">
+        <v>2028</v>
+      </c>
+      <c r="P58" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q58" s="6"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" s="11">
+        <v>44705</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="N59">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="6"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A60" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="14">
-        <v>44342</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="N54">
-        <v>1</v>
-      </c>
-      <c r="R54" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A55" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B55" s="11">
-        <v>44350</v>
-      </c>
-      <c r="P55" s="6"/>
-      <c r="R55" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A56" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B56" s="16">
-        <v>44469</v>
-      </c>
-      <c r="P56" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A57" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B57" s="16">
+      <c r="B60" s="16">
         <v>44712</v>
       </c>
-      <c r="P57" s="6"/>
-      <c r="R57" t="s">
+      <c r="P60" s="6"/>
+      <c r="R60" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A58" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" s="16">
-        <v>43091</v>
-      </c>
-      <c r="D58" t="s">
-        <v>215</v>
-      </c>
-      <c r="P58" s="6"/>
-      <c r="R58" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A59" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" s="14">
-        <v>43423</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="P59" s="6"/>
-      <c r="R59" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>60</v>
-      </c>
-      <c r="B60" s="18">
-        <v>43497</v>
-      </c>
-      <c r="G60">
-        <v>0.7</v>
-      </c>
-      <c r="H60">
-        <v>3</v>
-      </c>
-      <c r="R60" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>60</v>
-      </c>
-      <c r="B61" s="19">
-        <v>43634</v>
-      </c>
-      <c r="D61" t="s">
-        <v>220</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B61" s="11">
+        <v>44732</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
+      <c r="Q61" s="6"/>
       <c r="R61" t="s">
-        <v>219</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+      <c r="A62" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B62" s="14">
-        <v>44270</v>
-      </c>
-      <c r="D62" t="s">
-        <v>323</v>
-      </c>
-      <c r="E62"/>
+      <c r="B62" s="16" t="s">
+        <v>221</v>
+      </c>
       <c r="R62" t="s">
-        <v>324</v>
+        <v>222</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A63" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B63" s="16">
-        <v>44504</v>
-      </c>
-      <c r="D63" t="s">
-        <v>320</v>
-      </c>
-      <c r="P63" t="s">
-        <v>224</v>
+        <v>38</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="R63" t="s">
-        <v>223</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>87</v>
-      </c>
-      <c r="B64" s="11">
-        <v>44574</v>
-      </c>
-      <c r="G64">
-        <v>1.5</v>
-      </c>
-      <c r="H64">
-        <v>5</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="P64" s="6"/>
       <c r="R64" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A65" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B65" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="R65" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A66" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B66" s="14">
-        <v>43397</v>
-      </c>
-      <c r="P66" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A67" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B67" s="14">
-        <v>43419</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>47</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="P65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>109</v>
+      </c>
+      <c r="E66"/>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="P66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>75</v>
+      </c>
+      <c r="G67">
+        <v>0.3</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
       </c>
       <c r="N67">
-        <v>1</v>
-      </c>
-      <c r="P67" t="s">
-        <v>184</v>
-      </c>
-      <c r="R67" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A68" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" s="14">
-        <v>43518</v>
-      </c>
-      <c r="R68" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A69" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69" s="16">
-        <v>43850</v>
-      </c>
-      <c r="R69" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A70" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B70" s="14">
-        <v>44377</v>
-      </c>
-      <c r="R70" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A71" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B71" s="16">
-        <v>42283</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>110</v>
+      </c>
+      <c r="E68"/>
+      <c r="M68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>111</v>
+      </c>
+      <c r="E69"/>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>118</v>
+      </c>
+      <c r="E70"/>
+      <c r="M70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>112</v>
+      </c>
+      <c r="E71"/>
+      <c r="M71">
+        <v>0</v>
       </c>
       <c r="N71">
-        <v>1</v>
-      </c>
-      <c r="R71" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A72" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B72" s="11">
-        <v>42326</v>
-      </c>
-      <c r="R72" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A73" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B73" s="14">
-        <v>42996</v>
-      </c>
-      <c r="R73" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A74" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B74" s="14">
-        <v>43105</v>
-      </c>
-      <c r="R74" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A75" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B75" s="11">
-        <v>44179</v>
-      </c>
-      <c r="R75" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A76" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B76" s="14">
-        <v>44377</v>
-      </c>
-      <c r="R76" t="s">
-        <v>193</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>119</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>113</v>
+      </c>
+      <c r="E73"/>
+      <c r="M73">
+        <v>0</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>115</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>117</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>120</v>
+      </c>
+      <c r="E76"/>
+      <c r="M76">
+        <v>0</v>
+      </c>
+      <c r="N76">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:R76" xr:uid="{3D652218-3B78-4CB0-BA25-8DE344561C19}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R76">
-      <sortCondition ref="A1:A76"/>
+      <sortCondition ref="B1:B76"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="R37" r:id="rId1" display="https://global-factiva-com.gate3.library.lse.ac.uk/en/du/headlines.asp?napc=S&amp;searchText=(italy+or+italia)+and+(coal+or+lignite+or+carbone)+and+(202*+or+203*+or+204*)&amp;exclude=Recurring&amp;dateRangeMenu=custom&amp;dateFormat=dmy&amp;dateFrom=14102017&amp;dateTo=04112017&amp;sortBy=o&amp;currentSources=U%7csfreut%2csfeuac%2csfansa&amp;currentSourcesDesc=sc_u_sfreut%2cReuters+-+All+sources%3bsc_u_sfeuac%2cEurActiv+-+All+sources%3bsc_u_sfansa%2cANSA+-+All+sources&amp;searchLanguage=custom&amp;searchLang=&amp;dedupe=1&amp;srchuiver=2&amp;accountid=9LON003400&amp;namespace=16" xr:uid="{5D92F416-BAAC-4FB5-B839-9525CB830178}"/>
+    <hyperlink ref="R12" r:id="rId1" display="https://global-factiva-com.gate3.library.lse.ac.uk/en/du/headlines.asp?napc=S&amp;searchText=(italy+or+italia)+and+(coal+or+lignite+or+carbone)+and+(202*+or+203*+or+204*)&amp;exclude=Recurring&amp;dateRangeMenu=custom&amp;dateFormat=dmy&amp;dateFrom=14102017&amp;dateTo=04112017&amp;sortBy=o&amp;currentSources=U%7csfreut%2csfeuac%2csfansa&amp;currentSourcesDesc=sc_u_sfreut%2cReuters+-+All+sources%3bsc_u_sfeuac%2cEurActiv+-+All+sources%3bsc_u_sfansa%2cANSA+-+All+sources&amp;searchLanguage=custom&amp;searchLang=&amp;dedupe=1&amp;srchuiver=2&amp;accountid=9LON003400&amp;namespace=16" xr:uid="{5D92F416-BAAC-4FB5-B839-9525CB830178}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3614,10 +3617,10 @@
   <dimension ref="A1:O68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A71" sqref="A71"/>
+      <selection pane="bottomRight" activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4833,6 +4836,9 @@
       </c>
       <c r="L39">
         <v>1</v>
+      </c>
+      <c r="M39" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.45">
@@ -5698,7 +5704,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
add volume-based event study
</commit_message>
<xml_diff>
--- a/Other data/Coal phase out announcements.xlsx
+++ b/Other data/Coal phase out announcements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive - London School of Economics\Documents\LSE\GY489_Dissertation\LETS GO\Dissertation-Code-Data\Other data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861D108A-2728-44FC-93C7-5E9B26C836B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B564D1-77A1-4FF7-BE67-DFBFE770716B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2565,10 +2565,10 @@
   <dimension ref="A1:R76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2647,1183 +2647,1183 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="14">
-        <v>40872</v>
-      </c>
-      <c r="F2">
-        <v>2030</v>
-      </c>
-      <c r="R2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="14">
-        <v>41941</v>
-      </c>
-      <c r="D3" t="s">
-        <v>196</v>
-      </c>
-      <c r="G3">
-        <v>2.5</v>
-      </c>
-      <c r="H3">
-        <v>6</v>
-      </c>
-      <c r="L3">
+        <v>109</v>
+      </c>
+      <c r="E3"/>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="11">
+        <v>44480</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+      <c r="L4">
         <v>1</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="R3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="16">
-        <v>42283</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
+      <c r="O4" t="s">
+        <v>153</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>126</v>
+      </c>
       <c r="R4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="11">
-        <v>42326</v>
-      </c>
-      <c r="R5" t="s">
-        <v>189</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="15">
+        <v>44483</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="16">
-        <v>42636</v>
-      </c>
-      <c r="P6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6">
+        <v>0.3</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="14">
-        <v>42689</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="F7">
-        <v>2023</v>
-      </c>
-      <c r="G7">
-        <v>3.5</v>
-      </c>
-      <c r="H7">
-        <v>11</v>
-      </c>
-      <c r="K7" t="s">
-        <v>137</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="R7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+      <c r="E7"/>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="16">
-        <v>42697</v>
+        <v>84</v>
+      </c>
+      <c r="B8" s="15">
+        <v>44169</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8">
+        <v>2038</v>
       </c>
       <c r="G8">
-        <v>2.6</v>
+        <v>8.5</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="L8">
         <v>1</v>
       </c>
-      <c r="P8" s="6" t="s">
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="11">
+        <v>44568</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="14">
+        <v>40872</v>
+      </c>
+      <c r="F10">
+        <v>2030</v>
+      </c>
+      <c r="R10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="14">
+        <v>41941</v>
+      </c>
+      <c r="D11" t="s">
+        <v>196</v>
+      </c>
+      <c r="G11">
+        <v>2.5</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="P11" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="R8" t="s">
+      <c r="R11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="14">
+        <v>43055</v>
+      </c>
+      <c r="D12" t="s">
+        <v>198</v>
+      </c>
+      <c r="K12" t="s">
+        <v>199</v>
+      </c>
+      <c r="R12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13"/>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="16">
+        <v>42697</v>
+      </c>
+      <c r="G14">
+        <v>2.6</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="P14" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="R14" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B15" s="14">
         <v>42978</v>
       </c>
-      <c r="E9"/>
-      <c r="R9" t="s">
+      <c r="E15"/>
+      <c r="R15" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="14">
-        <v>42996</v>
-      </c>
-      <c r="R10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="15">
-        <v>43018</v>
-      </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="15">
-        <v>43032</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="R12" s="17" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="11">
-        <v>43049</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="R13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="14">
-        <v>43055</v>
-      </c>
-      <c r="D14" t="s">
-        <v>198</v>
-      </c>
-      <c r="K14" t="s">
-        <v>199</v>
-      </c>
-      <c r="R14" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="14">
-        <v>43055</v>
-      </c>
-      <c r="D15" t="s">
-        <v>211</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>12</v>
-      </c>
-      <c r="K15" t="s">
-        <v>138</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="P15" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="R15" t="s">
-        <v>212</v>
-      </c>
-    </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A16" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="16">
-        <v>43091</v>
-      </c>
-      <c r="D16" t="s">
-        <v>215</v>
-      </c>
-      <c r="P16" s="6"/>
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="14">
+        <v>43200</v>
+      </c>
+      <c r="E16"/>
       <c r="R16" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A17" s="4" t="s">
-        <v>8</v>
+      <c r="A17" t="s">
+        <v>24</v>
       </c>
       <c r="B17" s="14">
-        <v>43105</v>
-      </c>
+        <v>43391</v>
+      </c>
+      <c r="E17"/>
       <c r="R17" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="16">
-        <v>43169</v>
-      </c>
-      <c r="G18">
-        <v>0.9</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-      <c r="N18" t="s">
-        <v>52</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B18" s="14">
+        <v>43523</v>
+      </c>
+      <c r="E18"/>
       <c r="R18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B19" s="14">
-        <v>43200</v>
-      </c>
-      <c r="E19"/>
+        <v>42689</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19">
+        <v>2023</v>
+      </c>
+      <c r="G19">
+        <v>3.5</v>
+      </c>
+      <c r="H19">
+        <v>11</v>
+      </c>
+      <c r="K19" t="s">
+        <v>137</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="P19" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="R19" t="s">
-        <v>204</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="14">
-        <v>43238</v>
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="11">
+        <v>43357</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20">
+        <v>2038</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="6" t="s">
+        <v>108</v>
       </c>
       <c r="R20" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="11">
-        <v>43357</v>
+      <c r="B21" s="15">
+        <v>43491</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F21">
         <v>2038</v>
       </c>
+      <c r="G21">
+        <v>47.6</v>
+      </c>
+      <c r="H21">
+        <v>175</v>
+      </c>
       <c r="L21">
         <v>1</v>
       </c>
       <c r="N21">
         <v>1</v>
       </c>
-      <c r="Q21" s="6" t="s">
-        <v>108</v>
-      </c>
+      <c r="P21" s="6"/>
       <c r="R21" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="14">
-        <v>43391</v>
-      </c>
-      <c r="E22"/>
+        <v>61</v>
+      </c>
+      <c r="B22" s="11">
+        <v>43846</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22">
+        <v>2038</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="P22" s="6"/>
       <c r="R22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="14">
-        <v>43397</v>
-      </c>
-      <c r="P23" s="6" t="s">
-        <v>183</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="11">
+        <v>44015</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F23">
+        <v>2038</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="P23" s="6"/>
+      <c r="R23" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A24" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="14">
-        <v>43419</v>
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="11">
+        <v>44484</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24">
+        <v>2030</v>
       </c>
       <c r="N24">
         <v>1</v>
       </c>
-      <c r="P24" t="s">
-        <v>184</v>
+      <c r="P24" s="6" t="s">
+        <v>146</v>
       </c>
       <c r="R24" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A25" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="14">
-        <v>43423</v>
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="11">
+        <v>44705</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="P25" s="6"/>
-      <c r="R25" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="6"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" s="16">
-        <v>43424</v>
-      </c>
-      <c r="G26">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H26">
-        <v>4</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>194</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B26" s="11">
+        <v>44732</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="6"/>
       <c r="R26" t="s">
-        <v>207</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="15">
-        <v>43491</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F27">
-        <v>2038</v>
-      </c>
-      <c r="G27">
-        <v>47.6</v>
-      </c>
-      <c r="H27">
-        <v>175</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
+      <c r="B27" s="8" t="s">
+        <v>167</v>
       </c>
       <c r="P27" s="6"/>
       <c r="R27" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="18">
-        <v>43497</v>
-      </c>
-      <c r="G28">
-        <v>0.7</v>
-      </c>
-      <c r="H28">
-        <v>3</v>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="15">
+        <v>43731</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28">
+        <v>2028</v>
+      </c>
+      <c r="K28" t="s">
+        <v>148</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="R28" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A29" s="4" t="s">
-        <v>69</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>53</v>
       </c>
       <c r="B29" s="14">
-        <v>43518</v>
-      </c>
+        <v>44312</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F29">
+        <v>2025</v>
+      </c>
+      <c r="P29" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q29" s="6"/>
       <c r="R29" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B30" s="14">
-        <v>43523</v>
-      </c>
-      <c r="E30"/>
+        <v>44462</v>
+      </c>
       <c r="R30" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="19">
-        <v>43634</v>
-      </c>
-      <c r="D31" t="s">
-        <v>220</v>
-      </c>
-      <c r="R31" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="15">
-        <v>43731</v>
+      <c r="B31" s="16">
+        <v>44530</v>
+      </c>
+      <c r="Q31" s="6"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="14">
+        <v>44657</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="F32">
         <v>2028</v>
       </c>
-      <c r="K32" t="s">
-        <v>148</v>
-      </c>
-      <c r="N32">
-        <v>1</v>
-      </c>
-      <c r="P32" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="R32" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="P32" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q32" s="6"/>
+    </row>
+    <row r="33" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="16">
+        <v>43424</v>
+      </c>
+      <c r="G33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="P33" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="R33" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="14">
         <v>43731</v>
       </c>
-      <c r="Q33" s="6"/>
-      <c r="R33" t="s">
+      <c r="Q34" s="6"/>
+      <c r="R34" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="16">
-        <v>43731</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="14">
-        <v>43764</v>
+        <v>118</v>
       </c>
       <c r="E35"/>
-      <c r="R35" t="s">
-        <v>213</v>
+      <c r="M35">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A36" s="4" t="s">
-        <v>38</v>
+      <c r="A36" t="s">
+        <v>44</v>
       </c>
       <c r="B36" s="16">
-        <v>43802</v>
-      </c>
-      <c r="P36" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="11">
-        <v>43846</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="F37">
-        <v>2038</v>
+        <v>43169</v>
+      </c>
+      <c r="G36">
+        <v>0.9</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="N36" t="s">
+        <v>52</v>
+      </c>
+      <c r="R36" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="15">
+        <v>43032</v>
       </c>
       <c r="N37">
         <v>1</v>
       </c>
-      <c r="P37" s="6"/>
-      <c r="R37" t="s">
-        <v>159</v>
+      <c r="R37" s="17" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="16">
-        <v>43850</v>
+        <v>19</v>
+      </c>
+      <c r="B38" s="11">
+        <v>43049</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="R38" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="11">
-        <v>44015</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F39">
-        <v>2038</v>
-      </c>
-      <c r="N39">
-        <v>1</v>
-      </c>
-      <c r="P39" s="6"/>
-      <c r="R39" t="s">
-        <v>160</v>
+      <c r="A39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" s="16">
+        <v>43731</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="11">
-        <v>44099</v>
+        <v>112</v>
       </c>
       <c r="E40"/>
-      <c r="F40">
-        <v>2049</v>
-      </c>
-      <c r="G40">
-        <v>30.2</v>
-      </c>
-      <c r="H40">
-        <v>104</v>
-      </c>
-      <c r="R40" t="s">
-        <v>210</v>
+      <c r="M40">
+        <v>0</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" s="15">
-        <v>44169</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F41">
-        <v>2038</v>
-      </c>
-      <c r="G41">
-        <v>8.5</v>
-      </c>
-      <c r="H41">
-        <v>35</v>
-      </c>
-      <c r="L41">
-        <v>1</v>
+        <v>119</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
       </c>
       <c r="N41">
-        <v>1</v>
-      </c>
-      <c r="R41" t="s">
-        <v>156</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A42" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="11">
-        <v>44179</v>
-      </c>
-      <c r="R42" t="s">
-        <v>192</v>
+      <c r="A42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42"/>
+      <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="14">
-        <v>44270</v>
-      </c>
-      <c r="D43" t="s">
-        <v>319</v>
-      </c>
-      <c r="E43"/>
-      <c r="R43" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="14">
-        <v>44312</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F44">
-        <v>2025</v>
-      </c>
-      <c r="P44" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q44" s="6"/>
-      <c r="R44" t="s">
-        <v>179</v>
+        <v>117</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="14">
-        <v>44342</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="N45">
-        <v>1</v>
-      </c>
-      <c r="R45" t="s">
-        <v>175</v>
+        <v>38</v>
+      </c>
+      <c r="B45" s="16">
+        <v>42636</v>
+      </c>
+      <c r="P45" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A46" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="11">
-        <v>44350</v>
-      </c>
-      <c r="P46" s="6"/>
-      <c r="R46" t="s">
-        <v>175</v>
+        <v>38</v>
+      </c>
+      <c r="B46" s="15">
+        <v>43018</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="B47" s="14">
-        <v>44377</v>
+        <v>43238</v>
       </c>
       <c r="R47" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="14">
-        <v>44377</v>
-      </c>
-      <c r="R48" t="s">
-        <v>193</v>
+        <v>38</v>
+      </c>
+      <c r="B48" s="16">
+        <v>43802</v>
+      </c>
+      <c r="P48" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49" s="14">
-        <v>44462</v>
+      <c r="A49" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="R49" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A50" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B50" s="16">
-        <v>44469</v>
-      </c>
-      <c r="P50" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>120</v>
+      </c>
+      <c r="E50"/>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B51" s="11">
-        <v>44480</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="F51" t="s">
-        <v>127</v>
+        <v>44099</v>
+      </c>
+      <c r="E51"/>
+      <c r="F51">
+        <v>2049</v>
       </c>
       <c r="G51">
-        <v>5</v>
+        <v>30.2</v>
       </c>
       <c r="H51">
-        <v>15</v>
-      </c>
-      <c r="L51">
-        <v>1</v>
-      </c>
-      <c r="N51">
-        <v>1</v>
-      </c>
-      <c r="O51" t="s">
-        <v>153</v>
-      </c>
-      <c r="P51" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q51" s="6" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="R51" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52" s="15">
-        <v>44483</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F52" t="s">
-        <v>131</v>
+        <v>42</v>
+      </c>
+      <c r="B52" s="14">
+        <v>43055</v>
+      </c>
+      <c r="D52" t="s">
+        <v>211</v>
       </c>
       <c r="G52">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H52">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="K52" t="s">
+        <v>138</v>
       </c>
       <c r="L52">
         <v>1</v>
       </c>
-      <c r="N52">
-        <v>1</v>
+      <c r="P52" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="R52" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="11">
-        <v>44484</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="F53">
-        <v>2030</v>
-      </c>
-      <c r="N53">
-        <v>1</v>
-      </c>
-      <c r="P53" s="6" t="s">
-        <v>146</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B53" s="14">
+        <v>43764</v>
+      </c>
+      <c r="E53"/>
       <c r="R53" t="s">
-        <v>161</v>
+        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A54" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54" s="16">
-        <v>44504</v>
-      </c>
-      <c r="D54" t="s">
-        <v>316</v>
-      </c>
-      <c r="P54" t="s">
-        <v>224</v>
+        <v>76</v>
+      </c>
+      <c r="B54" s="14">
+        <v>44342</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
       </c>
       <c r="R54" t="s">
-        <v>223</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" s="16">
-        <v>44530</v>
-      </c>
-      <c r="Q55" s="6"/>
-    </row>
-    <row r="56" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>84</v>
-      </c>
-      <c r="B56" s="11">
-        <v>44568</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="N56">
-        <v>1</v>
-      </c>
-      <c r="R56" t="s">
-        <v>157</v>
+      <c r="A55" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="11">
+        <v>44350</v>
+      </c>
+      <c r="P55" s="6"/>
+      <c r="R55" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A56" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="16">
+        <v>44469</v>
+      </c>
+      <c r="P56" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>87</v>
-      </c>
-      <c r="B57" s="11">
-        <v>44574</v>
-      </c>
-      <c r="G57">
-        <v>1.5</v>
-      </c>
-      <c r="H57">
-        <v>5</v>
-      </c>
+      <c r="A57" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" s="16">
+        <v>44712</v>
+      </c>
+      <c r="P57" s="6"/>
       <c r="R57" t="s">
-        <v>225</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>53</v>
-      </c>
-      <c r="B58" s="14">
-        <v>44657</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="F58">
-        <v>2028</v>
-      </c>
-      <c r="P58" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q58" s="6"/>
+      <c r="A58" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="16">
+        <v>43091</v>
+      </c>
+      <c r="D58" t="s">
+        <v>215</v>
+      </c>
+      <c r="P58" s="6"/>
+      <c r="R58" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59" s="11">
-        <v>44705</v>
+      <c r="A59" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="14">
+        <v>43423</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="N59">
-        <v>1</v>
-      </c>
-      <c r="Q59" s="6"/>
+        <v>217</v>
+      </c>
+      <c r="P59" s="6"/>
+      <c r="R59" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A60" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B60" s="16">
-        <v>44712</v>
-      </c>
-      <c r="P60" s="6"/>
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" s="18">
+        <v>43497</v>
+      </c>
+      <c r="G60">
+        <v>0.7</v>
+      </c>
+      <c r="H60">
+        <v>3</v>
+      </c>
       <c r="R60" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>61</v>
-      </c>
-      <c r="B61" s="11">
-        <v>44732</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="N61">
-        <v>1</v>
-      </c>
-      <c r="Q61" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="B61" s="19">
+        <v>43634</v>
+      </c>
+      <c r="D61" t="s">
+        <v>220</v>
+      </c>
       <c r="R61" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A62" s="4" t="s">
+      <c r="A62" t="s">
         <v>87</v>
       </c>
-      <c r="B62" s="16" t="s">
-        <v>221</v>
-      </c>
+      <c r="B62" s="14">
+        <v>44270</v>
+      </c>
+      <c r="D62" t="s">
+        <v>319</v>
+      </c>
+      <c r="E62"/>
       <c r="R62" t="s">
-        <v>222</v>
+        <v>320</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A63" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B63" s="16" t="s">
-        <v>173</v>
+        <v>87</v>
+      </c>
+      <c r="B63" s="16">
+        <v>44504</v>
+      </c>
+      <c r="D63" t="s">
+        <v>316</v>
+      </c>
+      <c r="P63" t="s">
+        <v>224</v>
       </c>
       <c r="R63" t="s">
-        <v>181</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>61</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="P64" s="6"/>
+        <v>87</v>
+      </c>
+      <c r="B64" s="11">
+        <v>44574</v>
+      </c>
+      <c r="G64">
+        <v>1.5</v>
+      </c>
+      <c r="H64">
+        <v>5</v>
+      </c>
       <c r="R64" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>47</v>
-      </c>
-      <c r="N65">
-        <v>0</v>
-      </c>
-      <c r="P65" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>109</v>
-      </c>
-      <c r="E66"/>
-      <c r="M66">
-        <v>0</v>
-      </c>
-      <c r="P66" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>75</v>
-      </c>
-      <c r="G67">
-        <v>0.3</v>
-      </c>
-      <c r="H67">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A65" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="R65" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A66" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B66" s="14">
+        <v>43397</v>
+      </c>
+      <c r="P66" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A67" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B67" s="14">
+        <v>43419</v>
+      </c>
+      <c r="N67">
         <v>1</v>
       </c>
-      <c r="L67">
+      <c r="P67" t="s">
+        <v>184</v>
+      </c>
+      <c r="R67" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A68" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="14">
+        <v>43518</v>
+      </c>
+      <c r="R68" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A69" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" s="16">
+        <v>43850</v>
+      </c>
+      <c r="R69" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A70" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" s="14">
+        <v>44377</v>
+      </c>
+      <c r="R70" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A71" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" s="16">
+        <v>42283</v>
+      </c>
+      <c r="N71">
         <v>1</v>
       </c>
-      <c r="N67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>110</v>
-      </c>
-      <c r="E68"/>
-      <c r="M68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>111</v>
-      </c>
-      <c r="E69"/>
-      <c r="M69">
-        <v>0</v>
-      </c>
-      <c r="N69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>118</v>
-      </c>
-      <c r="E70"/>
-      <c r="M70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>112</v>
-      </c>
-      <c r="E71"/>
-      <c r="M71">
-        <v>0</v>
-      </c>
-      <c r="N71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>119</v>
-      </c>
-      <c r="M72">
-        <v>0</v>
-      </c>
-      <c r="N72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>113</v>
-      </c>
-      <c r="E73"/>
-      <c r="M73">
-        <v>0</v>
-      </c>
-      <c r="N73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>115</v>
-      </c>
-      <c r="M74">
-        <v>0</v>
-      </c>
-      <c r="N74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>117</v>
-      </c>
-      <c r="M75">
-        <v>0</v>
-      </c>
-      <c r="N75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>120</v>
-      </c>
-      <c r="E76"/>
-      <c r="M76">
-        <v>0</v>
-      </c>
-      <c r="N76">
-        <v>0</v>
+      <c r="R71" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A72" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B72" s="11">
+        <v>42326</v>
+      </c>
+      <c r="R72" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A73" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B73" s="14">
+        <v>42996</v>
+      </c>
+      <c r="R73" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A74" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="14">
+        <v>43105</v>
+      </c>
+      <c r="R74" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A75" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="11">
+        <v>44179</v>
+      </c>
+      <c r="R75" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A76" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B76" s="14">
+        <v>44377</v>
+      </c>
+      <c r="R76" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:R76" xr:uid="{3D652218-3B78-4CB0-BA25-8DE344561C19}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R76">
-      <sortCondition ref="B1:B76"/>
+      <sortCondition ref="A1:A76"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="R12" r:id="rId1" display="https://global-factiva-com.gate3.library.lse.ac.uk/en/du/headlines.asp?napc=S&amp;searchText=(italy+or+italia)+and+(coal+or+lignite+or+carbone)+and+(202*+or+203*+or+204*)&amp;exclude=Recurring&amp;dateRangeMenu=custom&amp;dateFormat=dmy&amp;dateFrom=14102017&amp;dateTo=04112017&amp;sortBy=o&amp;currentSources=U%7csfreut%2csfeuac%2csfansa&amp;currentSourcesDesc=sc_u_sfreut%2cReuters+-+All+sources%3bsc_u_sfeuac%2cEurActiv+-+All+sources%3bsc_u_sfansa%2cANSA+-+All+sources&amp;searchLanguage=custom&amp;searchLang=&amp;dedupe=1&amp;srchuiver=2&amp;accountid=9LON003400&amp;namespace=16" xr:uid="{5D92F416-BAAC-4FB5-B839-9525CB830178}"/>
+    <hyperlink ref="R37" r:id="rId1" display="https://global-factiva-com.gate3.library.lse.ac.uk/en/du/headlines.asp?napc=S&amp;searchText=(italy+or+italia)+and+(coal+or+lignite+or+carbone)+and+(202*+or+203*+or+204*)&amp;exclude=Recurring&amp;dateRangeMenu=custom&amp;dateFormat=dmy&amp;dateFrom=14102017&amp;dateTo=04112017&amp;sortBy=o&amp;currentSources=U%7csfreut%2csfeuac%2csfansa&amp;currentSourcesDesc=sc_u_sfreut%2cReuters+-+All+sources%3bsc_u_sfeuac%2cEurActiv+-+All+sources%3bsc_u_sfansa%2cANSA+-+All+sources&amp;searchLanguage=custom&amp;searchLang=&amp;dedupe=1&amp;srchuiver=2&amp;accountid=9LON003400&amp;namespace=16" xr:uid="{5D92F416-BAAC-4FB5-B839-9525CB830178}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -3835,10 +3835,10 @@
   <dimension ref="A1:Q68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M44" sqref="M44"/>
+      <selection pane="bottomRight" activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
small changes output msfe
</commit_message>
<xml_diff>
--- a/Other data/Coal phase out announcements.xlsx
+++ b/Other data/Coal phase out announcements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive - London School of Economics\Documents\LSE\GY489_Dissertation\LETS GO\Dissertation-Code-Data\Other data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED31F893-5F57-4996-9867-0DEAE314B613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6465F57A-C621-4D4D-AB83-47E5867B9B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="453">
   <si>
     <t>Country</t>
   </si>
@@ -1426,6 +1426,12 @@
   </si>
   <si>
     <t>https://global-factiva-com.gate3.library.lse.ac.uk/en/du/headlines.asp?napc=S&amp;searchText=(%22united+kingdom%22+or+uk+or+xxxx)+and+(coal+or+lignite+or+xxxxxx+or+xxxxxxx)+and+(2025+or+leak)&amp;exclude=Recurring&amp;dateRangeMenu=custom&amp;dateFormat=dmy&amp;dateFrom=08112014&amp;dateTo=28112015&amp;sortBy=o&amp;currentSources=U%7csfreut%2csfeuac%2csfft%2csfbbc&amp;currentSourcesDesc=sc_u_sfreut%2cReuters+-+All+sources%3bsc_u_sfeuac%2cEurActiv+-+All+sources%3bsc_u_sfft%2cFinancial+Times+(Available+through+Third+Party+Subscription+Services)+-+All+sources%3bsc_u_sfbbc%2cBBC+-+All+sources&amp;searchLanguage=custom&amp;searchLang=&amp;dedupe=1&amp;srchuiver=2&amp;accountid=9LON003400&amp;namespace=16</t>
+  </si>
+  <si>
+    <t>cancellation not mentioned in leaked draft</t>
+  </si>
+  <si>
+    <t>Five beneficiary Member States opt to transfer additional allowances to the Modernisation Fund (europa.eu)</t>
   </si>
 </sst>
 </file>
@@ -3906,19 +3912,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CCC5DF-E81D-45C6-92D8-92AE6A0AD22C}">
-  <dimension ref="A1:S68"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A51" sqref="A51"/>
+      <selection pane="bottomRight" activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.06640625" customWidth="1"/>
+    <col min="2" max="2" width="16.19921875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="36.73046875" style="4" customWidth="1"/>
     <col min="5" max="7" width="21.46484375" customWidth="1"/>
@@ -4660,69 +4666,47 @@
         <v>61</v>
       </c>
       <c r="B21" s="21">
-        <v>43808</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
+        <v>43781</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="H21" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" t="s">
-        <v>412</v>
-      </c>
-      <c r="K21" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+        <v>451</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>61</v>
       </c>
-      <c r="B22" s="10">
-        <v>43846</v>
+      <c r="B22" s="21">
+        <v>43808</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E22">
-        <v>2038</v>
+        <v>343</v>
       </c>
       <c r="H22" t="s">
-        <v>258</v>
+        <v>50</v>
       </c>
       <c r="I22" t="s">
-        <v>231</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="N22" t="s">
-        <v>52</v>
-      </c>
-      <c r="O22" t="s">
-        <v>290</v>
-      </c>
-      <c r="Q22" s="4"/>
-      <c r="R22" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.45">
+        <v>412</v>
+      </c>
+      <c r="K22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="21">
-        <v>44015</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
+      <c r="B23" s="10">
+        <v>43846</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23">
         <v>2038</v>
@@ -4730,21 +4714,21 @@
       <c r="H23" t="s">
         <v>258</v>
       </c>
+      <c r="I23" t="s">
+        <v>231</v>
+      </c>
       <c r="K23" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>413</v>
-      </c>
-      <c r="M23" s="13" t="s">
-        <v>414</v>
+        <v>268</v>
       </c>
       <c r="N23" t="s">
-        <v>287</v>
+        <v>52</v>
+      </c>
+      <c r="O23" t="s">
+        <v>290</v>
       </c>
       <c r="Q23" s="4"/>
       <c r="R23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.45">
@@ -4752,133 +4736,131 @@
         <v>61</v>
       </c>
       <c r="B24" s="21">
-        <v>44484</v>
-      </c>
-      <c r="C24" t="s">
-        <v>295</v>
+        <v>44015</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E24">
-        <v>2030</v>
+        <v>2038</v>
       </c>
       <c r="H24" t="s">
         <v>258</v>
       </c>
-      <c r="J24" t="s">
-        <v>416</v>
-      </c>
-      <c r="K24" t="s">
-        <v>259</v>
+      <c r="K24" s="13" t="s">
+        <v>269</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>415</v>
+        <v>413</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>414</v>
       </c>
       <c r="N24" t="s">
-        <v>289</v>
-      </c>
-      <c r="Q24" s="4" t="s">
-        <v>288</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="Q24" s="4"/>
       <c r="R24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="12">
-        <v>44705</v>
+      <c r="B25" s="21">
+        <v>44484</v>
+      </c>
+      <c r="C25" t="s">
+        <v>295</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+      <c r="E25">
+        <v>2030</v>
       </c>
       <c r="H25" t="s">
         <v>258</v>
       </c>
-      <c r="I25" t="s">
-        <v>418</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>275</v>
+      <c r="J25" t="s">
+        <v>416</v>
+      </c>
+      <c r="K25" t="s">
+        <v>259</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>276</v>
+        <v>415</v>
       </c>
       <c r="N25" t="s">
-        <v>286</v>
+        <v>289</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="R25" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="21">
-        <v>44732</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
+      <c r="B26" s="12">
+        <v>44705</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H26" t="s">
         <v>258</v>
       </c>
       <c r="I26" t="s">
-        <v>292</v>
-      </c>
-      <c r="J26" t="s">
-        <v>417</v>
-      </c>
-      <c r="K26" t="s">
-        <v>259</v>
+        <v>418</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>276</v>
       </c>
       <c r="N26" t="s">
-        <v>291</v>
-      </c>
-      <c r="R26" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="23">
-        <v>43731</v>
+        <v>61</v>
+      </c>
+      <c r="B27" s="21">
+        <v>44732</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27">
-        <v>2028</v>
+        <v>145</v>
       </c>
       <c r="H27" t="s">
         <v>258</v>
       </c>
       <c r="I27" t="s">
-        <v>229</v>
+        <v>292</v>
+      </c>
+      <c r="J27" t="s">
+        <v>417</v>
       </c>
       <c r="K27" t="s">
         <v>259</v>
       </c>
       <c r="N27" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q27" s="4" t="s">
-        <v>166</v>
+        <v>291</v>
       </c>
       <c r="R27" t="s">
-        <v>165</v>
-      </c>
-      <c r="S27" t="s">
-        <v>437</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
@@ -4886,54 +4868,60 @@
         <v>53</v>
       </c>
       <c r="B28" s="23">
-        <v>44312</v>
+        <v>43731</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>349</v>
+        <v>147</v>
       </c>
       <c r="E28">
-        <v>2025</v>
+        <v>2028</v>
       </c>
       <c r="H28" t="s">
         <v>258</v>
       </c>
       <c r="I28" t="s">
-        <v>297</v>
+        <v>229</v>
       </c>
       <c r="K28" t="s">
         <v>259</v>
       </c>
       <c r="N28" t="s">
-        <v>298</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>150</v>
+        <v>300</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="R28" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="S28" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.45">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>53</v>
       </c>
       <c r="B29" s="23">
-        <v>44462</v>
+        <v>44312</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>299</v>
+        <v>349</v>
+      </c>
+      <c r="E29">
+        <v>2025</v>
       </c>
       <c r="H29" t="s">
-        <v>52</v>
+        <v>258</v>
+      </c>
+      <c r="I29" t="s">
+        <v>297</v>
       </c>
       <c r="K29" t="s">
         <v>259</v>
@@ -4941,179 +4929,173 @@
       <c r="N29" t="s">
         <v>298</v>
       </c>
+      <c r="Q29" t="s">
+        <v>150</v>
+      </c>
       <c r="R29" t="s">
-        <v>178</v>
+        <v>179</v>
+      </c>
+      <c r="S29" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="12">
-        <v>44530</v>
+      <c r="B30" s="23">
+        <v>44462</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>299</v>
       </c>
       <c r="H30" t="s">
         <v>52</v>
       </c>
       <c r="K30" t="s">
-        <v>258</v>
-      </c>
-      <c r="N30">
-        <v>0</v>
+        <v>259</v>
+      </c>
+      <c r="N30" t="s">
+        <v>298</v>
+      </c>
+      <c r="R30" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="12">
+        <v>44530</v>
+      </c>
+      <c r="H31" t="s">
+        <v>52</v>
+      </c>
+      <c r="K31" t="s">
+        <v>258</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="10">
         <v>44657</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>0</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>2028</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H32" t="s">
         <v>258</v>
       </c>
-      <c r="K31" s="13" t="s">
+      <c r="K32" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N32" t="s">
         <v>52</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="Q32" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="23">
-        <v>43424</v>
-      </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="E32">
-        <v>2030</v>
-      </c>
-      <c r="F32">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G32">
-        <v>4</v>
-      </c>
-      <c r="H32" t="s">
-        <v>50</v>
-      </c>
-      <c r="I32" t="s">
-        <v>419</v>
-      </c>
-      <c r="K32" t="s">
-        <v>259</v>
-      </c>
-      <c r="N32" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q32" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="R32" t="s">
-        <v>207</v>
-      </c>
-      <c r="S32" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="10">
-        <v>43731</v>
+      <c r="B33" s="23">
+        <v>43424</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>301</v>
+        <v>279</v>
       </c>
       <c r="E33">
         <v>2030</v>
       </c>
+      <c r="F33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G33">
+        <v>4</v>
+      </c>
       <c r="H33" t="s">
-        <v>258</v>
+        <v>50</v>
       </c>
       <c r="I33" t="s">
-        <v>252</v>
+        <v>419</v>
       </c>
       <c r="K33" t="s">
         <v>259</v>
       </c>
       <c r="N33" t="s">
-        <v>52</v>
+        <v>300</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>194</v>
       </c>
       <c r="R33" t="s">
-        <v>208</v>
+        <v>207</v>
+      </c>
+      <c r="S33" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="22">
-        <v>43032</v>
+        <v>56</v>
+      </c>
+      <c r="B34" s="10">
+        <v>43731</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>301</v>
       </c>
       <c r="E34">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="H34" t="s">
         <v>258</v>
       </c>
-      <c r="J34" t="s">
-        <v>420</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>260</v>
+      <c r="I34" t="s">
+        <v>252</v>
+      </c>
+      <c r="K34" t="s">
+        <v>259</v>
       </c>
       <c r="N34" t="s">
-        <v>300</v>
-      </c>
-      <c r="P34" t="s">
-        <v>442</v>
-      </c>
-      <c r="R34" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="S34" t="s">
-        <v>441</v>
+        <v>52</v>
+      </c>
+      <c r="R34" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>19</v>
       </c>
-      <c r="B35" s="7">
-        <v>43049</v>
+      <c r="B35" s="22">
+        <v>43032</v>
       </c>
       <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>169</v>
+        <v>1</v>
       </c>
       <c r="E35">
         <v>2025</v>
@@ -5121,263 +5103,254 @@
       <c r="H35" t="s">
         <v>258</v>
       </c>
-      <c r="I35" t="s">
-        <v>408</v>
+      <c r="J35" t="s">
+        <v>420</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="L35" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N35" t="s">
-        <v>52</v>
-      </c>
-      <c r="R35" t="s">
-        <v>170</v>
+        <v>300</v>
+      </c>
+      <c r="P35" t="s">
+        <v>442</v>
+      </c>
+      <c r="R35" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="S35" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="12">
-        <v>43731</v>
+      <c r="B36" s="7">
+        <v>43049</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36">
+        <v>2025</v>
       </c>
       <c r="H36" t="s">
         <v>258</v>
       </c>
       <c r="I36" t="s">
-        <v>230</v>
-      </c>
-      <c r="K36" t="s">
-        <v>259</v>
-      </c>
-      <c r="N36">
-        <v>0</v>
+        <v>408</v>
+      </c>
+      <c r="K36" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="N36" t="s">
+        <v>52</v>
+      </c>
+      <c r="R36" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="23">
-        <v>42636</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>303</v>
+        <v>19</v>
+      </c>
+      <c r="B37" s="12">
+        <v>43731</v>
       </c>
       <c r="H37" t="s">
-        <v>50</v>
+        <v>258</v>
+      </c>
+      <c r="I37" t="s">
+        <v>230</v>
       </c>
       <c r="K37" t="s">
         <v>259</v>
       </c>
-      <c r="N37" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="N37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="22">
-        <v>43018</v>
+      <c r="B38" s="23">
+        <v>42636</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="E38">
-        <v>2030</v>
+        <v>303</v>
       </c>
       <c r="H38" t="s">
-        <v>258</v>
-      </c>
-      <c r="J38" t="s">
-        <v>422</v>
+        <v>50</v>
       </c>
       <c r="K38" t="s">
         <v>259</v>
       </c>
-      <c r="L38" s="13" t="s">
-        <v>421</v>
-      </c>
-      <c r="N38">
-        <v>1</v>
-      </c>
-      <c r="O38" t="s">
-        <v>350</v>
-      </c>
-      <c r="S38" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="N38" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="23">
-        <v>43238</v>
+      <c r="B39" s="22">
+        <v>43018</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>304</v>
+        <v>302</v>
+      </c>
+      <c r="E39">
+        <v>2030</v>
       </c>
       <c r="H39" t="s">
         <v>258</v>
       </c>
-      <c r="K39" s="13" t="s">
-        <v>262</v>
+      <c r="J39" t="s">
+        <v>422</v>
+      </c>
+      <c r="K39" t="s">
+        <v>259</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="N39" t="s">
-        <v>305</v>
-      </c>
-      <c r="R39" t="s">
-        <v>180</v>
+        <v>421</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39" t="s">
+        <v>350</v>
+      </c>
+      <c r="S39" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="12">
-        <v>43802</v>
+      <c r="B40" s="23">
+        <v>43238</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>304</v>
       </c>
       <c r="H40" t="s">
-        <v>52</v>
-      </c>
-      <c r="I40" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="K40" s="13" t="s">
-        <v>423</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>171</v>
+        <v>262</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="N40" t="s">
+        <v>305</v>
+      </c>
+      <c r="R40" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>173</v>
+      <c r="B41" s="12">
+        <v>43802</v>
+      </c>
+      <c r="H41" t="s">
+        <v>52</v>
+      </c>
+      <c r="I41" t="s">
+        <v>250</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>423</v>
       </c>
       <c r="N41">
         <v>0</v>
       </c>
-      <c r="R41" t="s">
+      <c r="Q41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="R42" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A42" s="20" t="s">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A43" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="21">
+      <c r="B43" s="21">
         <v>44099</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <v>1</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="E42">
+      <c r="E43">
         <v>2049</v>
       </c>
-      <c r="F42">
+      <c r="F43">
         <v>30.2</v>
       </c>
-      <c r="G42">
+      <c r="G43">
         <v>104</v>
-      </c>
-      <c r="H42" t="s">
-        <v>258</v>
-      </c>
-      <c r="K42" t="s">
-        <v>259</v>
-      </c>
-      <c r="N42" t="s">
-        <v>49</v>
-      </c>
-      <c r="R42" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="12">
-        <v>43055</v>
-      </c>
-      <c r="C43" t="s">
-        <v>211</v>
-      </c>
-      <c r="F43">
-        <v>2</v>
-      </c>
-      <c r="G43">
-        <v>12</v>
       </c>
       <c r="H43" t="s">
         <v>258</v>
       </c>
-      <c r="I43" t="s">
-        <v>249</v>
-      </c>
       <c r="K43" t="s">
-        <v>258</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
-      </c>
-      <c r="P43" t="s">
-        <v>445</v>
-      </c>
-      <c r="Q43" s="4" t="s">
-        <v>134</v>
+        <v>259</v>
+      </c>
+      <c r="N43" t="s">
+        <v>49</v>
       </c>
       <c r="R43" t="s">
-        <v>212</v>
-      </c>
-      <c r="S43" t="s">
-        <v>444</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="23">
+      <c r="B44" s="12">
         <v>43055</v>
       </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
-        <v>309</v>
-      </c>
-      <c r="E44" s="4">
-        <v>2030</v>
+      <c r="C44" t="s">
+        <v>211</v>
       </c>
       <c r="F44">
         <v>2</v>
@@ -5389,25 +5362,25 @@
         <v>258</v>
       </c>
       <c r="I44" t="s">
-        <v>138</v>
-      </c>
-      <c r="K44" s="13" t="s">
-        <v>424</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="M44" s="13" t="s">
-        <v>261</v>
-      </c>
-      <c r="N44" t="s">
-        <v>300</v>
+        <v>249</v>
+      </c>
+      <c r="K44" t="s">
+        <v>258</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="P44" t="s">
+        <v>445</v>
       </c>
       <c r="Q44" s="4" t="s">
         <v>134</v>
       </c>
       <c r="R44" t="s">
         <v>212</v>
+      </c>
+      <c r="S44" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="45" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
@@ -5415,77 +5388,92 @@
         <v>42</v>
       </c>
       <c r="B45" s="23">
-        <v>43764</v>
-      </c>
-      <c r="C45" t="s">
-        <v>49</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="E45">
-        <v>2023</v>
+        <v>43055</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>309</v>
+      </c>
+      <c r="E45" s="4">
+        <v>2030</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>12</v>
       </c>
       <c r="H45" t="s">
         <v>258</v>
       </c>
+      <c r="I45" t="s">
+        <v>138</v>
+      </c>
       <c r="K45" s="13" t="s">
-        <v>267</v>
+        <v>424</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="M45" s="13" t="s">
+        <v>261</v>
       </c>
       <c r="N45" t="s">
-        <v>298</v>
+        <v>300</v>
+      </c>
+      <c r="Q45" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="R45" t="s">
-        <v>213</v>
-      </c>
-      <c r="S45" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.45">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B46" s="23">
-        <v>44342</v>
+        <v>43764</v>
       </c>
       <c r="C46" t="s">
         <v>49</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>176</v>
+        <v>308</v>
       </c>
       <c r="E46">
-        <v>2032</v>
+        <v>2023</v>
       </c>
       <c r="H46" t="s">
         <v>258</v>
       </c>
       <c r="K46" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="L46" s="13" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="N46" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="R46" t="s">
-        <v>175</v>
+        <v>213</v>
+      </c>
+      <c r="S46" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="21">
-        <v>44350</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
+      <c r="B47" s="23">
+        <v>44342</v>
+      </c>
+      <c r="C47" t="s">
+        <v>49</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>310</v>
+        <v>176</v>
       </c>
       <c r="E47">
         <v>2032</v>
@@ -5494,75 +5482,83 @@
         <v>258</v>
       </c>
       <c r="K47" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="L47" s="13" t="s">
         <v>273</v>
       </c>
       <c r="N47" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q47" s="4"/>
+        <v>285</v>
+      </c>
       <c r="R47" t="s">
         <v>175</v>
-      </c>
-      <c r="S47" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>76</v>
       </c>
-      <c r="B48" s="23">
-        <v>44469</v>
-      </c>
-      <c r="C48" t="s">
-        <v>52</v>
+      <c r="B48" s="21">
+        <v>44350</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E48">
         <v>2032</v>
       </c>
       <c r="H48" t="s">
-        <v>50</v>
-      </c>
-      <c r="K48" t="s">
         <v>258</v>
       </c>
-      <c r="Q48" t="s">
-        <v>174</v>
+      <c r="K48" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="N48" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q48" s="4"/>
+      <c r="R48" t="s">
+        <v>175</v>
+      </c>
+      <c r="S48" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="12">
-        <v>44712</v>
+      <c r="B49" s="23">
+        <v>44469</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E49">
+        <v>2032</v>
       </c>
       <c r="H49" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K49" t="s">
         <v>258</v>
       </c>
-      <c r="N49">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="4"/>
-      <c r="R49" t="s">
-        <v>177</v>
+      <c r="Q49" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B50" s="12">
-        <v>43091</v>
-      </c>
-      <c r="C50" t="s">
-        <v>215</v>
+        <v>44712</v>
       </c>
       <c r="H50" t="s">
         <v>52</v>
@@ -5575,286 +5571,272 @@
       </c>
       <c r="Q50" s="4"/>
       <c r="R50" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="23">
-        <v>43423</v>
-      </c>
-      <c r="C51">
+      <c r="B51" s="12">
+        <v>43091</v>
+      </c>
+      <c r="C51" t="s">
+        <v>215</v>
+      </c>
+      <c r="H51" t="s">
+        <v>52</v>
+      </c>
+      <c r="K51" t="s">
+        <v>258</v>
+      </c>
+      <c r="N51">
         <v>0</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="E51">
-        <v>2023</v>
-      </c>
-      <c r="H51" t="s">
-        <v>258</v>
-      </c>
-      <c r="I51" t="s">
-        <v>340</v>
-      </c>
-      <c r="K51" t="s">
-        <v>259</v>
       </c>
       <c r="Q51" s="4"/>
       <c r="R51" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.45">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>60</v>
       </c>
-      <c r="B52" s="12">
-        <v>43497</v>
-      </c>
-      <c r="F52">
-        <v>0.7</v>
-      </c>
-      <c r="G52">
-        <v>3</v>
+      <c r="B52" s="23">
+        <v>43423</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="E52">
+        <v>2023</v>
       </c>
       <c r="H52" t="s">
-        <v>52</v>
+        <v>258</v>
+      </c>
+      <c r="I52" t="s">
+        <v>340</v>
       </c>
       <c r="K52" t="s">
-        <v>258</v>
-      </c>
-      <c r="N52">
-        <v>0</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="Q52" s="4"/>
       <c r="R52" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="23">
-        <v>43634</v>
-      </c>
-      <c r="C53" t="s">
-        <v>49</v>
-      </c>
-      <c r="D53" t="s">
-        <v>220</v>
-      </c>
-      <c r="E53">
-        <v>2023</v>
+      <c r="B53" s="12">
+        <v>43497</v>
+      </c>
+      <c r="F53">
+        <v>0.7</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
       </c>
       <c r="H53" t="s">
+        <v>52</v>
+      </c>
+      <c r="K53" t="s">
         <v>258</v>
       </c>
-      <c r="K53" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="L53" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="N53" t="s">
-        <v>315</v>
-      </c>
-      <c r="P53" t="s">
-        <v>449</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>314</v>
+      <c r="N53">
+        <v>0</v>
       </c>
       <c r="R53" t="s">
-        <v>219</v>
-      </c>
-      <c r="S53" t="s">
-        <v>448</v>
+        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="B54" s="23">
-        <v>44270</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
+        <v>43634</v>
+      </c>
+      <c r="C54" t="s">
+        <v>49</v>
       </c>
       <c r="D54" t="s">
-        <v>321</v>
+        <v>220</v>
       </c>
       <c r="E54">
-        <v>2033</v>
+        <v>2023</v>
       </c>
       <c r="H54" t="s">
-        <v>52</v>
-      </c>
-      <c r="K54" t="s">
-        <v>259</v>
+        <v>258</v>
+      </c>
+      <c r="K54" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="N54" t="s">
-        <v>49</v>
+        <v>315</v>
+      </c>
+      <c r="P54" t="s">
+        <v>449</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>314</v>
       </c>
       <c r="R54" t="s">
-        <v>320</v>
+        <v>219</v>
+      </c>
+      <c r="S54" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>87</v>
       </c>
-      <c r="B55" s="24">
-        <v>44502</v>
+      <c r="B55" s="23">
+        <v>44270</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>321</v>
+      </c>
+      <c r="E55">
+        <v>2033</v>
       </c>
       <c r="H55" t="s">
         <v>52</v>
       </c>
-      <c r="I55" t="s">
-        <v>251</v>
-      </c>
       <c r="K55" t="s">
         <v>259</v>
       </c>
-      <c r="N55">
-        <v>0</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>224</v>
+      <c r="N55" t="s">
+        <v>49</v>
       </c>
       <c r="R55" t="s">
-        <v>223</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>87</v>
       </c>
-      <c r="B56" s="23">
-        <v>44574</v>
-      </c>
-      <c r="C56" t="s">
-        <v>49</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="E56">
-        <v>2033</v>
-      </c>
-      <c r="F56">
-        <v>1.5</v>
-      </c>
-      <c r="G56">
-        <v>5</v>
+      <c r="B56" s="24">
+        <v>44502</v>
       </c>
       <c r="H56" t="s">
-        <v>258</v>
+        <v>52</v>
+      </c>
+      <c r="I56" t="s">
+        <v>251</v>
       </c>
       <c r="K56" t="s">
         <v>259</v>
       </c>
-      <c r="N56" t="s">
-        <v>51</v>
+      <c r="N56">
+        <v>0</v>
       </c>
       <c r="Q56" t="s">
-        <v>318</v>
+        <v>224</v>
       </c>
       <c r="R56" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>87</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="23">
+        <v>44574</v>
+      </c>
+      <c r="C57" t="s">
+        <v>49</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E57">
+        <v>2033</v>
+      </c>
+      <c r="F57">
+        <v>1.5</v>
+      </c>
+      <c r="G57">
+        <v>5</v>
+      </c>
+      <c r="H57" t="s">
+        <v>258</v>
+      </c>
+      <c r="K57" t="s">
+        <v>259</v>
+      </c>
+      <c r="N57" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>318</v>
+      </c>
+      <c r="R57" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="N57">
+      <c r="N58">
         <v>0</v>
       </c>
-      <c r="R57" t="s">
+      <c r="R58" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>69</v>
-      </c>
-      <c r="B58" s="23">
-        <v>43397</v>
-      </c>
-      <c r="C58" t="s">
-        <v>51</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="H58" t="s">
-        <v>258</v>
-      </c>
-      <c r="K58" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q58" s="4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>69</v>
       </c>
       <c r="B59" s="23">
-        <v>43419</v>
+        <v>43397</v>
       </c>
       <c r="C59" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="E59">
-        <v>2030</v>
+        <v>322</v>
       </c>
       <c r="H59" t="s">
         <v>258</v>
       </c>
-      <c r="I59" t="s">
-        <v>339</v>
-      </c>
-      <c r="K59" t="s">
-        <v>259</v>
-      </c>
-      <c r="N59" t="s">
-        <v>323</v>
+      <c r="K59" s="13" t="s">
+        <v>263</v>
       </c>
       <c r="Q59" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="R59" t="s">
-        <v>182</v>
-      </c>
-      <c r="S59" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>69</v>
       </c>
       <c r="B60" s="23">
-        <v>43518</v>
+        <v>43419</v>
       </c>
       <c r="C60" t="s">
         <v>49</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E60">
         <v>2030</v>
@@ -5863,36 +5845,51 @@
         <v>258</v>
       </c>
       <c r="I60" t="s">
-        <v>227</v>
-      </c>
-      <c r="K60" s="13" t="s">
-        <v>264</v>
+        <v>339</v>
+      </c>
+      <c r="K60" t="s">
+        <v>259</v>
+      </c>
+      <c r="N60" t="s">
+        <v>323</v>
+      </c>
+      <c r="Q60" s="4" t="s">
+        <v>325</v>
       </c>
       <c r="R60" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.45">
+        <v>182</v>
+      </c>
+      <c r="S60" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>69</v>
       </c>
-      <c r="B61" s="12">
-        <v>43850</v>
+      <c r="B61" s="23">
+        <v>43518</v>
+      </c>
+      <c r="C61" t="s">
+        <v>49</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E61">
+        <v>2030</v>
       </c>
       <c r="H61" t="s">
-        <v>52</v>
+        <v>258</v>
       </c>
       <c r="I61" t="s">
-        <v>232</v>
-      </c>
-      <c r="K61" t="s">
-        <v>258</v>
-      </c>
-      <c r="N61">
-        <v>0</v>
+        <v>227</v>
+      </c>
+      <c r="K61" s="13" t="s">
+        <v>264</v>
       </c>
       <c r="R61" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.45">
@@ -5900,97 +5897,88 @@
         <v>69</v>
       </c>
       <c r="B62" s="12">
-        <v>44377</v>
+        <v>43850</v>
       </c>
       <c r="H62" t="s">
+        <v>52</v>
+      </c>
+      <c r="I62" t="s">
+        <v>232</v>
+      </c>
+      <c r="K62" t="s">
         <v>258</v>
-      </c>
-      <c r="I62" t="s">
-        <v>233</v>
-      </c>
-      <c r="K62" s="13" t="s">
-        <v>274</v>
       </c>
       <c r="N62">
         <v>0</v>
       </c>
       <c r="R62" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>8</v>
-      </c>
-      <c r="B63" s="23">
-        <v>42283</v>
-      </c>
-      <c r="C63" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="E63">
-        <v>2023</v>
+        <v>69</v>
+      </c>
+      <c r="B63" s="12">
+        <v>44377</v>
       </c>
       <c r="H63" t="s">
-        <v>50</v>
-      </c>
-      <c r="K63" t="s">
-        <v>259</v>
-      </c>
-      <c r="N63" t="s">
-        <v>285</v>
+        <v>258</v>
+      </c>
+      <c r="I63" t="s">
+        <v>233</v>
+      </c>
+      <c r="K63" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
       </c>
       <c r="R63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="21">
-        <v>42326</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
+      <c r="B64" s="23">
+        <v>42283</v>
+      </c>
+      <c r="C64" t="s">
+        <v>49</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E64">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="H64" t="s">
-        <v>258</v>
+        <v>50</v>
       </c>
       <c r="K64" t="s">
         <v>259</v>
       </c>
       <c r="N64" t="s">
-        <v>328</v>
+        <v>285</v>
       </c>
       <c r="R64" t="s">
-        <v>189</v>
-      </c>
-      <c r="S64" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.45">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="10">
-        <v>42996</v>
+      <c r="B65" s="21">
+        <v>42326</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E65">
         <v>2025</v>
@@ -6002,24 +5990,27 @@
         <v>259</v>
       </c>
       <c r="N65" t="s">
-        <v>52</v>
+        <v>328</v>
       </c>
       <c r="R65" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.45">
+        <v>189</v>
+      </c>
+      <c r="S65" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>8</v>
       </c>
-      <c r="B66" s="23">
-        <v>43105</v>
+      <c r="B66" s="10">
+        <v>42996</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E66">
         <v>2025</v>
@@ -6030,123 +6021,153 @@
       <c r="K66" t="s">
         <v>259</v>
       </c>
-      <c r="L66" s="13" t="s">
-        <v>426</v>
-      </c>
       <c r="N66" t="s">
-        <v>331</v>
+        <v>52</v>
       </c>
       <c r="R66" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="21">
-        <v>44179</v>
+      <c r="B67" s="23">
+        <v>43105</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E67">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="H67" t="s">
         <v>258</v>
       </c>
-      <c r="K67" s="13" t="s">
-        <v>270</v>
+      <c r="K67" t="s">
+        <v>259</v>
       </c>
       <c r="L67" s="13" t="s">
-        <v>271</v>
+        <v>426</v>
       </c>
       <c r="N67" t="s">
-        <v>334</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="R67" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.45">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>8</v>
       </c>
-      <c r="B68" s="12">
-        <v>44377</v>
+      <c r="B68" s="21">
+        <v>44179</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E68">
+        <v>2024</v>
       </c>
       <c r="H68" t="s">
         <v>258</v>
       </c>
-      <c r="I68" t="s">
+      <c r="K68" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="L68" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="N68" t="s">
+        <v>334</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>335</v>
+      </c>
+      <c r="R68" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B69" s="12">
+        <v>44377</v>
+      </c>
+      <c r="H69" t="s">
+        <v>258</v>
+      </c>
+      <c r="I69" t="s">
         <v>234</v>
       </c>
-      <c r="K68" s="13" t="s">
+      <c r="K69" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="N68">
+      <c r="N69">
         <v>0</v>
       </c>
-      <c r="R68" t="s">
+      <c r="R69" t="s">
         <v>193</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:S1" xr:uid="{D2CCC5DF-E81D-45C6-92D8-92AE6A0AD22C}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S68">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S69">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="R34" r:id="rId1" display="https://global-factiva-com.gate3.library.lse.ac.uk/en/du/headlines.asp?napc=S&amp;searchText=(italy+or+italia)+and+(coal+or+lignite+or+carbone)+and+(202*+or+203*+or+204*)&amp;exclude=Recurring&amp;dateRangeMenu=custom&amp;dateFormat=dmy&amp;dateFrom=14102017&amp;dateTo=04112017&amp;sortBy=o&amp;currentSources=U%7csfreut%2csfeuac%2csfansa&amp;currentSourcesDesc=sc_u_sfreut%2cReuters+-+All+sources%3bsc_u_sfeuac%2cEurActiv+-+All+sources%3bsc_u_sfansa%2cANSA+-+All+sources&amp;searchLanguage=custom&amp;searchLang=&amp;dedupe=1&amp;srchuiver=2&amp;accountid=9LON003400&amp;namespace=16" xr:uid="{505B5FEE-A6F5-47CB-9917-E30704A91A4C}"/>
+    <hyperlink ref="R35" r:id="rId1" display="https://global-factiva-com.gate3.library.lse.ac.uk/en/du/headlines.asp?napc=S&amp;searchText=(italy+or+italia)+and+(coal+or+lignite+or+carbone)+and+(202*+or+203*+or+204*)&amp;exclude=Recurring&amp;dateRangeMenu=custom&amp;dateFormat=dmy&amp;dateFrom=14102017&amp;dateTo=04112017&amp;sortBy=o&amp;currentSources=U%7csfreut%2csfeuac%2csfansa&amp;currentSourcesDesc=sc_u_sfreut%2cReuters+-+All+sources%3bsc_u_sfeuac%2cEurActiv+-+All+sources%3bsc_u_sfansa%2cANSA+-+All+sources&amp;searchLanguage=custom&amp;searchLang=&amp;dedupe=1&amp;srchuiver=2&amp;accountid=9LON003400&amp;namespace=16" xr:uid="{505B5FEE-A6F5-47CB-9917-E30704A91A4C}"/>
     <hyperlink ref="K6" r:id="rId2" display="https://ec.europa.eu/clima/news-your-voice/news/update-preparatory-steps-auctioning-phase-3-allowances-2011-11-25_en" xr:uid="{E0BDB423-56EA-44F0-A54A-0F5B4F2A2147}"/>
     <hyperlink ref="L6" r:id="rId3" display="https://ec.europa.eu/clima/news-your-voice/news/enhancing-eu-rules-monitoring-greenhouse-gas-emissions-2011-11-23_en" xr:uid="{9BD80364-5CA2-43DB-B2CC-0E03E8DA4A0C}"/>
     <hyperlink ref="K7" r:id="rId4" display="https://ec.europa.eu/clima/news-your-voice/news/european-commission-adopts-carbon-leakage-list-period-2015-2019-2014-10-27_en" xr:uid="{A6A17CE0-740F-4D5D-B313-5A7D344A91EA}"/>
     <hyperlink ref="L7" r:id="rId5" display="https://ec.europa.eu/clima/news-your-voice/news/updated-information-exchange-and-international-credit-use-eu-ets-2014-11-04_en" xr:uid="{8247D59B-1565-4720-B464-3B76D4306051}"/>
-    <hyperlink ref="K34" r:id="rId6" display="https://ec.europa.eu/clima/news-your-voice/news/commission-proposes-safeguard-measures-eu-emissions-trading-system-2017-10-24_en" xr:uid="{0DD0FCDC-28E2-41DE-B6F4-45CBD31C5107}"/>
-    <hyperlink ref="K35" r:id="rId7" display="https://ec.europa.eu/clima/news-your-voice/news/updated-information-exchange-and-international-credit-use-eu-ets-2017-11-06_en" xr:uid="{13CCF2E4-4BEB-447B-B73C-69BAB51FDDF4}"/>
-    <hyperlink ref="L35" r:id="rId8" display="https://ec.europa.eu/clima/news-your-voice/news/eu-emissions-trading-system-landmark-agreement-between-parliament-and-council-delivers-eus-2017-11-09_en" xr:uid="{454861F8-3E39-4C29-A4AA-465B15683294}"/>
-    <hyperlink ref="K39" r:id="rId9" display="https://ec.europa.eu/clima/news-your-voice/news/ets-market-stability-reserve-will-start-reducing-auction-volume-almost-265-million-allowances-over-2018-05-15_en" xr:uid="{C721078D-42C8-4E8F-A645-8D1BD1241E6C}"/>
-    <hyperlink ref="K58" r:id="rId10" display="https://ec.europa.eu/clima/news-your-voice/news/emissions-trading-commission-adopts-amendment-ets-auctioning-regulation-2018-10-30_en" xr:uid="{1DA6063C-C717-4DBA-BA11-FA42D50774A1}"/>
-    <hyperlink ref="K60" r:id="rId11" display="https://ec.europa.eu/clima/news-your-voice/news/towards-climate-neutral-europe-eu-invests-over-eu10bn-innovative-clean-technologies-2019-02-26_en" xr:uid="{507015DA-B303-49DD-BE42-8DA9AF07D7DC}"/>
+    <hyperlink ref="K35" r:id="rId6" display="https://ec.europa.eu/clima/news-your-voice/news/commission-proposes-safeguard-measures-eu-emissions-trading-system-2017-10-24_en" xr:uid="{0DD0FCDC-28E2-41DE-B6F4-45CBD31C5107}"/>
+    <hyperlink ref="K36" r:id="rId7" display="https://ec.europa.eu/clima/news-your-voice/news/updated-information-exchange-and-international-credit-use-eu-ets-2017-11-06_en" xr:uid="{13CCF2E4-4BEB-447B-B73C-69BAB51FDDF4}"/>
+    <hyperlink ref="L36" r:id="rId8" display="https://ec.europa.eu/clima/news-your-voice/news/eu-emissions-trading-system-landmark-agreement-between-parliament-and-council-delivers-eus-2017-11-09_en" xr:uid="{454861F8-3E39-4C29-A4AA-465B15683294}"/>
+    <hyperlink ref="K40" r:id="rId9" display="https://ec.europa.eu/clima/news-your-voice/news/ets-market-stability-reserve-will-start-reducing-auction-volume-almost-265-million-allowances-over-2018-05-15_en" xr:uid="{C721078D-42C8-4E8F-A645-8D1BD1241E6C}"/>
+    <hyperlink ref="K59" r:id="rId10" display="https://ec.europa.eu/clima/news-your-voice/news/emissions-trading-commission-adopts-amendment-ets-auctioning-regulation-2018-10-30_en" xr:uid="{1DA6063C-C717-4DBA-BA11-FA42D50774A1}"/>
+    <hyperlink ref="K61" r:id="rId11" display="https://ec.europa.eu/clima/news-your-voice/news/towards-climate-neutral-europe-eu-invests-over-eu10bn-innovative-clean-technologies-2019-02-26_en" xr:uid="{507015DA-B303-49DD-BE42-8DA9AF07D7DC}"/>
     <hyperlink ref="K14" r:id="rId12" display="https://ec.europa.eu/clima/news-your-voice/news/towards-climate-neutral-europe-eu-invests-over-eu10bn-innovative-clean-technologies-2019-02-26_en" xr:uid="{F695F6A8-94CC-4324-881A-6C6ADE693EA0}"/>
-    <hyperlink ref="K53" r:id="rId13" display="https://ec.europa.eu/clima/news-your-voice/news/updated-information-exchange-and-international-credit-use-eu-ets-2019-06-19_en" xr:uid="{A71B360B-E82C-443B-A0BC-C4F1B76F9882}"/>
-    <hyperlink ref="L53" r:id="rId14" display="https://ec.europa.eu/clima/news-your-voice/news/polands-2020-auction-volume-include-allowances-not-used-power-sector-modernisation-2019-06-12_en" xr:uid="{415A5C0B-1796-4A12-9A96-39DA2523F414}"/>
-    <hyperlink ref="K45" r:id="rId15" display="https://ec.europa.eu/clima/news-your-voice/news/adoption-regulation-adjustments-free-allocation-emission-allowances-due-activity-level-changes-2019-10-31_en" xr:uid="{F8C2477A-A966-4A33-B989-ABEB3FD073BF}"/>
-    <hyperlink ref="K22" r:id="rId16" display="https://ec.europa.eu/clima/news-your-voice/news/commission-publishes-status-update-new-entrants-reserve-2020-01-15_en" xr:uid="{ABCA4C5C-168F-4911-A05E-3E193BB0607F}"/>
-    <hyperlink ref="K23" r:id="rId17" display="https://ec.europa.eu/clima/news-your-voice/news/2020-revised-auction-calendars-published-2020-07-01_en" xr:uid="{9D566DF6-E071-4458-A5B6-59D0E48FBF3A}"/>
+    <hyperlink ref="K54" r:id="rId13" display="https://ec.europa.eu/clima/news-your-voice/news/updated-information-exchange-and-international-credit-use-eu-ets-2019-06-19_en" xr:uid="{A71B360B-E82C-443B-A0BC-C4F1B76F9882}"/>
+    <hyperlink ref="L54" r:id="rId14" display="https://ec.europa.eu/clima/news-your-voice/news/polands-2020-auction-volume-include-allowances-not-used-power-sector-modernisation-2019-06-12_en" xr:uid="{415A5C0B-1796-4A12-9A96-39DA2523F414}"/>
+    <hyperlink ref="K46" r:id="rId15" display="https://ec.europa.eu/clima/news-your-voice/news/adoption-regulation-adjustments-free-allocation-emission-allowances-due-activity-level-changes-2019-10-31_en" xr:uid="{F8C2477A-A966-4A33-B989-ABEB3FD073BF}"/>
+    <hyperlink ref="K23" r:id="rId16" display="https://ec.europa.eu/clima/news-your-voice/news/commission-publishes-status-update-new-entrants-reserve-2020-01-15_en" xr:uid="{ABCA4C5C-168F-4911-A05E-3E193BB0607F}"/>
+    <hyperlink ref="K24" r:id="rId17" display="https://ec.europa.eu/clima/news-your-voice/news/2020-revised-auction-calendars-published-2020-07-01_en" xr:uid="{9D566DF6-E071-4458-A5B6-59D0E48FBF3A}"/>
     <hyperlink ref="K4" r:id="rId18" display="https://ec.europa.eu/clima/news-your-voice/news/draft-implementing-regulation-determining-revised-benchmark-values-period-2021-2025-open-4-week-2020-12-08_en" xr:uid="{19E0304F-6616-473B-A894-D0B7F9DBC892}"/>
-    <hyperlink ref="K67" r:id="rId19" display="https://ec.europa.eu/clima/news-your-voice/news/draft-implementing-regulation-determining-revised-benchmark-values-period-2021-2025-open-4-week-2020-12-08_en" xr:uid="{658F0735-A061-4C52-B67E-F6B04D42BB54}"/>
-    <hyperlink ref="L67" r:id="rId20" display="https://ec.europa.eu/clima/news-your-voice/news/further-information-start-phase-4-eu-ets-2021-emission-allowances-be-issued-aircraft-operators-and-2020-12-11_en" xr:uid="{687C8CA1-0617-4C04-B1E2-3A6EE9FA542A}"/>
-    <hyperlink ref="K46" r:id="rId21" display="https://ec.europa.eu/clima/news-your-voice/news/updated-information-exchange-and-international-credits-use-eu-ets-2021-05-25_en" xr:uid="{786141D5-4E60-47E5-868D-0BC2E5D732A1}"/>
-    <hyperlink ref="L46" r:id="rId22" display="https://ec.europa.eu/clima/news-your-voice/news/commission-adopts-uniform-cross-sectoral-correction-factor-be-applied-free-allocation-2021-2025-eu-2021-05-31_en" xr:uid="{727E1C4B-1C90-4B4F-B840-392DA92B4D85}"/>
-    <hyperlink ref="K47" r:id="rId23" display="https://ec.europa.eu/clima/news-your-voice/news/commission-adopts-uniform-cross-sectoral-correction-factor-be-applied-free-allocation-2021-2025-eu-2021-05-31_en" xr:uid="{229EEBB8-9D9F-4092-B53F-78A789BC03EF}"/>
-    <hyperlink ref="K62" r:id="rId24" display="https://ec.europa.eu/clima/news-your-voice/news/commission-publishes-national-allocation-tables-member-states-eu-ets-stationary-installations-2021-06-29_en" xr:uid="{89D453DE-89FB-4B15-9C24-8E5340DED0FD}"/>
-    <hyperlink ref="K68" r:id="rId25" display="https://ec.europa.eu/clima/news-your-voice/news/commission-publishes-national-allocation-tables-member-states-eu-ets-stationary-installations-2021-06-29_en" xr:uid="{E19D2B34-612B-4770-9952-A0724072D571}"/>
-    <hyperlink ref="K25" r:id="rId26" display="https://ec.europa.eu/clima/news-your-voice/news/revised-2022-auction-calendar-general-allowances-published-2022-05-19_en" xr:uid="{D6A0CCD9-573F-4ABD-A090-B97A1BD04FAE}"/>
-    <hyperlink ref="L25" r:id="rId27" display="https://ec.europa.eu/commission/presscorner/detail/en/ip_22_3131" xr:uid="{EBAADABC-FD35-40D8-894F-A1A7B431C0BC}"/>
+    <hyperlink ref="K68" r:id="rId19" display="https://ec.europa.eu/clima/news-your-voice/news/draft-implementing-regulation-determining-revised-benchmark-values-period-2021-2025-open-4-week-2020-12-08_en" xr:uid="{658F0735-A061-4C52-B67E-F6B04D42BB54}"/>
+    <hyperlink ref="L68" r:id="rId20" display="https://ec.europa.eu/clima/news-your-voice/news/further-information-start-phase-4-eu-ets-2021-emission-allowances-be-issued-aircraft-operators-and-2020-12-11_en" xr:uid="{687C8CA1-0617-4C04-B1E2-3A6EE9FA542A}"/>
+    <hyperlink ref="K47" r:id="rId21" display="https://ec.europa.eu/clima/news-your-voice/news/updated-information-exchange-and-international-credits-use-eu-ets-2021-05-25_en" xr:uid="{786141D5-4E60-47E5-868D-0BC2E5D732A1}"/>
+    <hyperlink ref="L47" r:id="rId22" display="https://ec.europa.eu/clima/news-your-voice/news/commission-adopts-uniform-cross-sectoral-correction-factor-be-applied-free-allocation-2021-2025-eu-2021-05-31_en" xr:uid="{727E1C4B-1C90-4B4F-B840-392DA92B4D85}"/>
+    <hyperlink ref="K48" r:id="rId23" display="https://ec.europa.eu/clima/news-your-voice/news/commission-adopts-uniform-cross-sectoral-correction-factor-be-applied-free-allocation-2021-2025-eu-2021-05-31_en" xr:uid="{229EEBB8-9D9F-4092-B53F-78A789BC03EF}"/>
+    <hyperlink ref="K63" r:id="rId24" display="https://ec.europa.eu/clima/news-your-voice/news/commission-publishes-national-allocation-tables-member-states-eu-ets-stationary-installations-2021-06-29_en" xr:uid="{89D453DE-89FB-4B15-9C24-8E5340DED0FD}"/>
+    <hyperlink ref="K69" r:id="rId25" display="https://ec.europa.eu/clima/news-your-voice/news/commission-publishes-national-allocation-tables-member-states-eu-ets-stationary-installations-2021-06-29_en" xr:uid="{E19D2B34-612B-4770-9952-A0724072D571}"/>
+    <hyperlink ref="K26" r:id="rId26" display="https://ec.europa.eu/clima/news-your-voice/news/revised-2022-auction-calendar-general-allowances-published-2022-05-19_en" xr:uid="{D6A0CCD9-573F-4ABD-A090-B97A1BD04FAE}"/>
+    <hyperlink ref="L26" r:id="rId27" display="https://ec.europa.eu/commission/presscorner/detail/en/ip_22_3131" xr:uid="{EBAADABC-FD35-40D8-894F-A1A7B431C0BC}"/>
     <hyperlink ref="L4" r:id="rId28" display="https://ec.europa.eu/clima/news-your-voice/news/further-information-start-phase-4-eu-ets-2021-emission-allowances-be-issued-aircraft-operators-and-2020-12-11_en" xr:uid="{EDEA86E0-E622-447C-A19C-FB5362C65735}"/>
     <hyperlink ref="M7" r:id="rId29" display="https://ec.europa.eu/clima/news-your-voice/news/eu-leaders-agree-2030-climate-and-energy-goals-2014-10-24_en" xr:uid="{091C0239-D1B9-4526-BD63-97C9DEA7A648}"/>
-    <hyperlink ref="L23" r:id="rId30" display="https://ec.europa.eu/clima/news-your-voice/news/financing-energy-transition-commission-puts-eu14-billion-fund-modernise-energy-sectors-10-member-2020-07-09_en" xr:uid="{5B8F9CC5-B7D3-4BC4-A650-352814C687BC}"/>
-    <hyperlink ref="M23" r:id="rId31" display="https://ec.europa.eu/clima/news-your-voice/news/boosting-eus-green-recovery-commission-invests-eu-1-billion-innovative-clean-technology-projects-2020-07-03_en" xr:uid="{C0A7BD83-7044-4ED1-818F-46B46744F552}"/>
-    <hyperlink ref="L24" r:id="rId32" display="https://ec.europa.eu/commission/presscorner/detail/en/ip_21_6042" xr:uid="{8854F8D5-0532-4F0E-91C7-60C67286654D}"/>
-    <hyperlink ref="L38" r:id="rId33" display="https://ec.europa.eu/clima/news-your-voice/news/eu-member-states-agree-negotiating-position-key-2030-climate-policy-proposals-2017-10-13_en" xr:uid="{70D0D58B-B7F9-45A6-A335-5B8700139411}"/>
-    <hyperlink ref="K40" r:id="rId34" display="https://ec.europa.eu/clima/news-your-voice/news/member-states-emission-reduction-targets-2021-2030-adopted-2018-05-14_en" xr:uid="{26A50BE7-AD06-4B9A-9645-E4391F452CFF}"/>
-    <hyperlink ref="L39" r:id="rId35" display="https://ec.europa.eu/clima/news-your-voice/news/ets-market-stability-reserve-will-start-reducing-auction-volume-almost-265-million-allowances-over-2018-05-15_en" xr:uid="{C9572FEA-0976-472B-AAEC-D5F85E2EE313}"/>
-    <hyperlink ref="K44" r:id="rId36" display="https://ec.europa.eu/clima/news-your-voice/news/eu-and-switzerland-sign-agreement-link-emissions-trading-systems-2017-11-23_en" xr:uid="{D1F584D8-A9E6-4830-B87A-59072962FBDE}"/>
-    <hyperlink ref="L44" r:id="rId37" display="https://ec.europa.eu/clima/news-your-voice/news/un-climate-conference-makes-progress-paris-agreement-implementation-2017-11-18_en" xr:uid="{BEFA94A6-DDF4-4E95-A6FA-BCD766336BF9}"/>
-    <hyperlink ref="M44" r:id="rId38" display="https://ec.europa.eu/clima/news-your-voice/news/eu-emissions-trading-system-landmark-agreement-between-parliament-and-council-delivers-eus-2017-11-09_en" xr:uid="{BE6B9B42-B032-4671-BCB8-5AD6B033B4BC}"/>
-    <hyperlink ref="L66" r:id="rId39" display="https://ec.europa.eu/clima/news-your-voice/news/update-safeguard-measures-eu-emissions-trading-system-2018-following-adoption-uk-law-2018-01-08_en" xr:uid="{60C5A314-1D7C-4699-9335-84B9B95C6199}"/>
+    <hyperlink ref="L24" r:id="rId30" display="https://ec.europa.eu/clima/news-your-voice/news/financing-energy-transition-commission-puts-eu14-billion-fund-modernise-energy-sectors-10-member-2020-07-09_en" xr:uid="{5B8F9CC5-B7D3-4BC4-A650-352814C687BC}"/>
+    <hyperlink ref="M24" r:id="rId31" display="https://ec.europa.eu/clima/news-your-voice/news/boosting-eus-green-recovery-commission-invests-eu-1-billion-innovative-clean-technology-projects-2020-07-03_en" xr:uid="{C0A7BD83-7044-4ED1-818F-46B46744F552}"/>
+    <hyperlink ref="L25" r:id="rId32" display="https://ec.europa.eu/commission/presscorner/detail/en/ip_21_6042" xr:uid="{8854F8D5-0532-4F0E-91C7-60C67286654D}"/>
+    <hyperlink ref="L39" r:id="rId33" display="https://ec.europa.eu/clima/news-your-voice/news/eu-member-states-agree-negotiating-position-key-2030-climate-policy-proposals-2017-10-13_en" xr:uid="{70D0D58B-B7F9-45A6-A335-5B8700139411}"/>
+    <hyperlink ref="K41" r:id="rId34" display="https://ec.europa.eu/clima/news-your-voice/news/member-states-emission-reduction-targets-2021-2030-adopted-2018-05-14_en" xr:uid="{26A50BE7-AD06-4B9A-9645-E4391F452CFF}"/>
+    <hyperlink ref="L40" r:id="rId35" display="https://ec.europa.eu/clima/news-your-voice/news/ets-market-stability-reserve-will-start-reducing-auction-volume-almost-265-million-allowances-over-2018-05-15_en" xr:uid="{C9572FEA-0976-472B-AAEC-D5F85E2EE313}"/>
+    <hyperlink ref="K45" r:id="rId36" display="https://ec.europa.eu/clima/news-your-voice/news/eu-and-switzerland-sign-agreement-link-emissions-trading-systems-2017-11-23_en" xr:uid="{D1F584D8-A9E6-4830-B87A-59072962FBDE}"/>
+    <hyperlink ref="L45" r:id="rId37" display="https://ec.europa.eu/clima/news-your-voice/news/un-climate-conference-makes-progress-paris-agreement-implementation-2017-11-18_en" xr:uid="{BEFA94A6-DDF4-4E95-A6FA-BCD766336BF9}"/>
+    <hyperlink ref="M45" r:id="rId38" display="https://ec.europa.eu/clima/news-your-voice/news/eu-emissions-trading-system-landmark-agreement-between-parliament-and-council-delivers-eus-2017-11-09_en" xr:uid="{BE6B9B42-B032-4671-BCB8-5AD6B033B4BC}"/>
+    <hyperlink ref="L67" r:id="rId39" display="https://ec.europa.eu/clima/news-your-voice/news/update-safeguard-measures-eu-emissions-trading-system-2018-following-adoption-uk-law-2018-01-08_en" xr:uid="{60C5A314-1D7C-4699-9335-84B9B95C6199}"/>
+    <hyperlink ref="K21" r:id="rId40" display="https://ec.europa.eu/clima/news-your-voice/news/five-beneficiary-member-states-opt-transfer-additional-allowances-modernisation-fund-2019-11-08_en" xr:uid="{140E77F1-1C6A-42DC-AF8B-5C47B20828C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
 

</xml_diff>